<commit_message>
Implement ReportServices and ReportController for generating Info and B1 reports
</commit_message>
<xml_diff>
--- a/SeaEco.Server/wwwroot/reports/Rapporter.xlsx
+++ b/SeaEco.Server/wwwroot/reports/Rapporter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tetianaverkhalantseva/Documents/Bacheloroppgave/Sea Eco AS/Del2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tetianaverkhalantseva/RiderProjects/SeaEco/SeaEco.Server/wwwroot/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709951C0-B7C9-AB42-8CA5-0B3B0377C002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A9BA56-172C-8F41-82D3-C3B52A28DB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="186">
   <si>
     <t>St.nr.</t>
   </si>
@@ -605,9 +605,6 @@
     <t>Hardbunnsstasjoner</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -620,22 +617,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>SE25-BU-1</t>
-  </si>
-  <si>
     <t>Prosjekt:</t>
   </si>
   <si>
     <t>Dato:</t>
-  </si>
-  <si>
-    <t>29.08 og 16.09.2024</t>
-  </si>
-  <si>
-    <t>Feltdatoer</t>
-  </si>
-  <si>
-    <t>Prosjektet som inneholder f.eks 18 B-undersøkelser til hver stasjon</t>
   </si>
 </sst>
 </file>
@@ -1974,7 +1959,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="259">
+  <cellXfs count="258">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2447,13 +2432,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2703,6 +2681,10 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4806,8 +4788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9A826C-1207-43A0-B1E5-0610FD134460}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4819,35 +4801,27 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="166" t="s">
-        <v>186</v>
-      </c>
-      <c r="B1" s="174" t="s">
-        <v>185</v>
-      </c>
-      <c r="C1" s="175" t="s">
-        <v>190</v>
-      </c>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
+        <v>184</v>
+      </c>
+      <c r="B1" s="256"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="172"/>
+      <c r="H1" s="172"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="166" t="s">
-        <v>187</v>
-      </c>
-      <c r="B2" s="174" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" s="175" t="s">
-        <v>189</v>
-      </c>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
+        <v>185</v>
+      </c>
+      <c r="B2" s="257"/>
+      <c r="C2" s="257"/>
+      <c r="D2" s="257"/>
+      <c r="E2" s="172"/>
+      <c r="F2" s="172"/>
+      <c r="G2" s="172"/>
+      <c r="H2" s="172"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="166" t="s">
@@ -4861,41 +4835,31 @@
       <c r="A5" s="168" t="s">
         <v>163</v>
       </c>
-      <c r="B5" s="169">
-        <v>18</v>
-      </c>
+      <c r="B5" s="169"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="168" t="s">
         <v>166</v>
       </c>
-      <c r="B6" s="169">
-        <v>22</v>
-      </c>
+      <c r="B6" s="169"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="168" t="s">
         <v>179</v>
       </c>
-      <c r="B7" s="169">
-        <v>3</v>
-      </c>
+      <c r="B7" s="169"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="168" t="s">
         <v>164</v>
       </c>
-      <c r="B8" s="169">
-        <v>16</v>
-      </c>
+      <c r="B8" s="169"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="168" t="s">
         <v>165</v>
       </c>
-      <c r="B9" s="169">
-        <v>15</v>
-      </c>
+      <c r="B9" s="169"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="166" t="s">
@@ -4909,57 +4873,43 @@
       <c r="A12" s="170" t="s">
         <v>126</v>
       </c>
-      <c r="B12" s="169">
-        <v>0</v>
-      </c>
+      <c r="B12" s="169"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="170" t="s">
         <v>127</v>
       </c>
-      <c r="B13" s="169">
-        <v>12.5</v>
-      </c>
+      <c r="B13" s="169"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="170" t="s">
         <v>128</v>
       </c>
-      <c r="B14" s="169">
-        <v>15</v>
-      </c>
+      <c r="B14" s="169"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="170" t="s">
         <v>129</v>
       </c>
-      <c r="B15" s="169">
-        <v>1</v>
-      </c>
+      <c r="B15" s="169"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="170" t="s">
         <v>130</v>
       </c>
-      <c r="B16" s="169">
-        <v>0</v>
-      </c>
+      <c r="B16" s="169"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="170" t="s">
         <v>131</v>
       </c>
-      <c r="B17" s="169">
-        <v>0.5</v>
-      </c>
+      <c r="B17" s="169"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="170" t="s">
         <v>132</v>
       </c>
-      <c r="B18" s="169">
-        <v>3</v>
-      </c>
+      <c r="B18" s="169"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="166" t="s">
@@ -4976,45 +4926,29 @@
       <c r="A21" s="170" t="s">
         <v>173</v>
       </c>
-      <c r="B21" s="169">
-        <v>5</v>
-      </c>
-      <c r="C21" s="169">
-        <v>3</v>
-      </c>
+      <c r="B21" s="169"/>
+      <c r="C21" s="169"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="170" t="s">
         <v>174</v>
       </c>
-      <c r="B22" s="169">
-        <v>5</v>
-      </c>
-      <c r="C22" s="169" t="s">
-        <v>180</v>
-      </c>
+      <c r="B22" s="169"/>
+      <c r="C22" s="169"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="170" t="s">
         <v>175</v>
       </c>
-      <c r="B23" s="169">
-        <v>3</v>
-      </c>
-      <c r="C23" s="169" t="s">
-        <v>180</v>
-      </c>
+      <c r="B23" s="169"/>
+      <c r="C23" s="169"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="170" t="s">
         <v>176</v>
       </c>
-      <c r="B24" s="169">
-        <v>5</v>
-      </c>
-      <c r="C24" s="169" t="s">
-        <v>180</v>
-      </c>
+      <c r="B24" s="169"/>
+      <c r="C24" s="169"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="166" t="s">
@@ -5031,36 +4965,27 @@
       <c r="A27" s="170" t="s">
         <v>169</v>
       </c>
-      <c r="B27" s="169">
-        <v>2.78</v>
-      </c>
-      <c r="C27" s="173">
-        <v>3</v>
-      </c>
+      <c r="B27" s="169"/>
+      <c r="C27" s="169"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="170" t="s">
         <v>170</v>
       </c>
-      <c r="B28" s="169">
-        <v>1.26</v>
-      </c>
-      <c r="C28" s="172">
-        <v>2</v>
-      </c>
+      <c r="B28" s="169"/>
+      <c r="C28" s="169"/>
     </row>
     <row r="29" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="171" t="s">
         <v>171</v>
       </c>
-      <c r="B29" s="169">
-        <v>2.02</v>
-      </c>
-      <c r="C29" s="172">
-        <v>2</v>
-      </c>
+      <c r="B29" s="169"/>
+      <c r="C29" s="169"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5469,7 +5394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73EE1091-9F45-40A9-90F5-6AF0F1D8D5C5}">
   <dimension ref="A1:AC50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
@@ -5486,70 +5411,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A1" s="204" t="s">
+      <c r="A1" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="205"/>
-      <c r="C1" s="205"/>
+      <c r="B1" s="202"/>
+      <c r="C1" s="202"/>
       <c r="D1" s="4"/>
       <c r="E1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="206" t="s">
+      <c r="F1" s="203" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="206"/>
-      <c r="H1" s="206"/>
+      <c r="G1" s="203"/>
+      <c r="H1" s="203"/>
       <c r="I1" s="6"/>
       <c r="J1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="207" t="s">
+      <c r="K1" s="204" t="s">
         <v>112</v>
       </c>
-      <c r="L1" s="207"/>
+      <c r="L1" s="204"/>
       <c r="M1" s="7"/>
       <c r="N1" s="8"/>
-      <c r="P1" s="204" t="s">
+      <c r="P1" s="201" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="205"/>
-      <c r="R1" s="205"/>
+      <c r="Q1" s="202"/>
+      <c r="R1" s="202"/>
       <c r="S1" s="4"/>
       <c r="T1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="U1" s="206" t="s">
+      <c r="U1" s="203" t="s">
         <v>110</v>
       </c>
-      <c r="V1" s="206"/>
-      <c r="W1" s="206"/>
+      <c r="V1" s="203"/>
+      <c r="W1" s="203"/>
       <c r="X1" s="6"/>
       <c r="Y1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Z1" s="207" t="s">
+      <c r="Z1" s="204" t="s">
         <v>112</v>
       </c>
-      <c r="AA1" s="207"/>
+      <c r="AA1" s="204"/>
       <c r="AB1" s="7"/>
       <c r="AC1" s="8"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A2" s="218" t="s">
+      <c r="A2" s="215" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="219"/>
-      <c r="C2" s="219"/>
+      <c r="B2" s="216"/>
+      <c r="C2" s="216"/>
       <c r="D2" s="9"/>
       <c r="E2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="210" t="s">
+      <c r="F2" s="207" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="210"/>
-      <c r="H2" s="210"/>
+      <c r="G2" s="207"/>
+      <c r="H2" s="207"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10" t="s">
         <v>49</v>
@@ -5560,20 +5485,20 @@
       <c r="L2" s="10"/>
       <c r="M2" s="10"/>
       <c r="N2" s="12"/>
-      <c r="P2" s="208" t="s">
+      <c r="P2" s="205" t="s">
         <v>144</v>
       </c>
-      <c r="Q2" s="209"/>
-      <c r="R2" s="209"/>
+      <c r="Q2" s="206"/>
+      <c r="R2" s="206"/>
       <c r="S2" s="9"/>
       <c r="T2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="U2" s="210" t="s">
+      <c r="U2" s="207" t="s">
         <v>111</v>
       </c>
-      <c r="V2" s="210"/>
-      <c r="W2" s="210"/>
+      <c r="V2" s="207"/>
+      <c r="W2" s="207"/>
       <c r="X2" s="10"/>
       <c r="Y2" s="10" t="s">
         <v>49</v>
@@ -5586,59 +5511,59 @@
       <c r="AC2" s="12"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A3" s="211" t="s">
+      <c r="A3" s="208" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="213" t="s">
+      <c r="B3" s="210" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="213" t="s">
+      <c r="C3" s="210" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="191" t="s">
+      <c r="D3" s="188" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="191"/>
-      <c r="F3" s="191"/>
-      <c r="G3" s="191"/>
-      <c r="H3" s="191"/>
-      <c r="I3" s="191"/>
-      <c r="J3" s="191"/>
-      <c r="K3" s="191"/>
-      <c r="L3" s="191"/>
-      <c r="M3" s="191"/>
+      <c r="E3" s="188"/>
+      <c r="F3" s="188"/>
+      <c r="G3" s="188"/>
+      <c r="H3" s="188"/>
+      <c r="I3" s="188"/>
+      <c r="J3" s="188"/>
+      <c r="K3" s="188"/>
+      <c r="L3" s="188"/>
+      <c r="M3" s="188"/>
       <c r="N3" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="P3" s="211" t="s">
+      <c r="P3" s="208" t="s">
         <v>50</v>
       </c>
-      <c r="Q3" s="213" t="s">
+      <c r="Q3" s="210" t="s">
         <v>51</v>
       </c>
-      <c r="R3" s="213" t="s">
+      <c r="R3" s="210" t="s">
         <v>52</v>
       </c>
-      <c r="S3" s="191" t="s">
+      <c r="S3" s="188" t="s">
         <v>53</v>
       </c>
-      <c r="T3" s="191"/>
-      <c r="U3" s="191"/>
-      <c r="V3" s="191"/>
-      <c r="W3" s="191"/>
-      <c r="X3" s="191"/>
-      <c r="Y3" s="191"/>
-      <c r="Z3" s="191"/>
-      <c r="AA3" s="191"/>
-      <c r="AB3" s="191"/>
+      <c r="T3" s="188"/>
+      <c r="U3" s="188"/>
+      <c r="V3" s="188"/>
+      <c r="W3" s="188"/>
+      <c r="X3" s="188"/>
+      <c r="Y3" s="188"/>
+      <c r="Z3" s="188"/>
+      <c r="AA3" s="188"/>
+      <c r="AB3" s="188"/>
       <c r="AC3" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A4" s="212"/>
-      <c r="B4" s="214"/>
-      <c r="C4" s="214"/>
+      <c r="A4" s="209"/>
+      <c r="B4" s="211"/>
+      <c r="C4" s="211"/>
       <c r="D4" s="14">
         <v>1</v>
       </c>
@@ -5670,9 +5595,9 @@
         <v>10</v>
       </c>
       <c r="N4" s="15"/>
-      <c r="P4" s="212"/>
-      <c r="Q4" s="214"/>
-      <c r="R4" s="214"/>
+      <c r="P4" s="209"/>
+      <c r="Q4" s="211"/>
+      <c r="R4" s="211"/>
       <c r="S4" s="14">
         <v>11</v>
       </c>
@@ -5706,11 +5631,11 @@
       <c r="AC4" s="15"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A5" s="215" t="s">
+      <c r="A5" s="212" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="216"/>
-      <c r="C5" s="217"/>
+      <c r="B5" s="213"/>
+      <c r="C5" s="214"/>
       <c r="D5" s="16" t="s">
         <v>7</v>
       </c>
@@ -5742,11 +5667,11 @@
         <v>19</v>
       </c>
       <c r="N5" s="15"/>
-      <c r="P5" s="192" t="s">
+      <c r="P5" s="189" t="s">
         <v>55</v>
       </c>
-      <c r="Q5" s="193"/>
-      <c r="R5" s="194"/>
+      <c r="Q5" s="190"/>
+      <c r="R5" s="191"/>
       <c r="S5" s="16" t="s">
         <v>7</v>
       </c>
@@ -6137,69 +6062,69 @@
     </row>
     <row r="12" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
-      <c r="B12" s="195" t="s">
+      <c r="B12" s="192" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="195"/>
+      <c r="C12" s="192"/>
       <c r="D12" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="J12" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N12" s="15"/>
       <c r="P12" s="17"/>
-      <c r="Q12" s="195" t="s">
+      <c r="Q12" s="192" t="s">
         <v>66</v>
       </c>
-      <c r="R12" s="195"/>
+      <c r="R12" s="192"/>
       <c r="S12" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="U12" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="T12" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="V12" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="X12" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y12" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="Y12" s="1" t="s">
+      <c r="Z12" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="Z12" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="AA12" s="146"/>
       <c r="AB12" s="146"/>
@@ -6207,10 +6132,10 @@
     </row>
     <row r="13" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
-      <c r="B13" s="182" t="s">
+      <c r="B13" s="179" t="s">
         <v>172</v>
       </c>
-      <c r="C13" s="182"/>
+      <c r="C13" s="179"/>
       <c r="D13" s="33" t="s">
         <v>65</v>
       </c>
@@ -6225,12 +6150,12 @@
       <c r="M13" s="19"/>
       <c r="N13" s="15"/>
       <c r="P13" s="17"/>
-      <c r="Q13" s="182" t="s">
+      <c r="Q13" s="179" t="s">
         <v>172</v>
       </c>
-      <c r="R13" s="182"/>
+      <c r="R13" s="179"/>
       <c r="S13" s="151" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="T13" s="19"/>
       <c r="U13" s="19"/>
@@ -6262,10 +6187,10 @@
       <c r="J14" s="71">
         <v>14.33</v>
       </c>
-      <c r="K14" s="196" t="s">
+      <c r="K14" s="193" t="s">
         <v>69</v>
       </c>
-      <c r="L14" s="197"/>
+      <c r="L14" s="194"/>
       <c r="M14" s="73">
         <v>11.050666666666665</v>
       </c>
@@ -6288,10 +6213,10 @@
       <c r="Y14" s="36">
         <v>14.33</v>
       </c>
-      <c r="Z14" s="196" t="s">
+      <c r="Z14" s="193" t="s">
         <v>69</v>
       </c>
-      <c r="AA14" s="197"/>
+      <c r="AA14" s="194"/>
       <c r="AB14" s="153">
         <v>11.050666666666665</v>
       </c>
@@ -6316,10 +6241,10 @@
       <c r="J15" s="71">
         <v>161.1</v>
       </c>
-      <c r="K15" s="196" t="s">
+      <c r="K15" s="193" t="s">
         <v>72</v>
       </c>
-      <c r="L15" s="197"/>
+      <c r="L15" s="194"/>
       <c r="M15" s="74"/>
       <c r="N15" s="15"/>
       <c r="P15" s="17"/>
@@ -6340,10 +6265,10 @@
       <c r="Y15" s="36">
         <v>161.1</v>
       </c>
-      <c r="Z15" s="196" t="s">
+      <c r="Z15" s="193" t="s">
         <v>72</v>
       </c>
-      <c r="AA15" s="197"/>
+      <c r="AA15" s="194"/>
       <c r="AB15" s="152" t="s">
         <v>113</v>
       </c>
@@ -6383,7 +6308,7 @@
       <c r="A17" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="198" t="s">
+      <c r="B17" s="195" t="s">
         <v>74</v>
       </c>
       <c r="C17" s="39" t="s">
@@ -6423,7 +6348,7 @@
       <c r="P17" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="Q17" s="198" t="s">
+      <c r="Q17" s="195" t="s">
         <v>74</v>
       </c>
       <c r="R17" s="39" t="s">
@@ -6463,7 +6388,7 @@
     </row>
     <row r="18" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
-      <c r="B18" s="199"/>
+      <c r="B18" s="196"/>
       <c r="C18" s="44" t="s">
         <v>76</v>
       </c>
@@ -6499,7 +6424,7 @@
       </c>
       <c r="N18" s="15"/>
       <c r="P18" s="17"/>
-      <c r="Q18" s="199"/>
+      <c r="Q18" s="196"/>
       <c r="R18" s="44" t="s">
         <v>76</v>
       </c>
@@ -6537,7 +6462,7 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
-      <c r="B19" s="198" t="s">
+      <c r="B19" s="195" t="s">
         <v>77</v>
       </c>
       <c r="C19" s="39" t="s">
@@ -6575,7 +6500,7 @@
       </c>
       <c r="N19" s="15"/>
       <c r="P19" s="17"/>
-      <c r="Q19" s="198" t="s">
+      <c r="Q19" s="195" t="s">
         <v>77</v>
       </c>
       <c r="R19" s="39" t="s">
@@ -6615,7 +6540,7 @@
     </row>
     <row r="20" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
-      <c r="B20" s="199"/>
+      <c r="B20" s="196"/>
       <c r="C20" s="44" t="s">
         <v>79</v>
       </c>
@@ -6651,7 +6576,7 @@
       </c>
       <c r="N20" s="15"/>
       <c r="P20" s="17"/>
-      <c r="Q20" s="199"/>
+      <c r="Q20" s="196"/>
       <c r="R20" s="44" t="s">
         <v>79</v>
       </c>
@@ -6689,7 +6614,7 @@
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" s="17"/>
-      <c r="B21" s="198" t="s">
+      <c r="B21" s="195" t="s">
         <v>80</v>
       </c>
       <c r="C21" s="39" t="s">
@@ -6727,7 +6652,7 @@
       </c>
       <c r="N21" s="15"/>
       <c r="P21" s="17"/>
-      <c r="Q21" s="198" t="s">
+      <c r="Q21" s="195" t="s">
         <v>80</v>
       </c>
       <c r="R21" s="39" t="s">
@@ -6767,7 +6692,7 @@
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" s="17"/>
-      <c r="B22" s="200"/>
+      <c r="B22" s="197"/>
       <c r="C22" s="28" t="s">
         <v>82</v>
       </c>
@@ -6803,7 +6728,7 @@
       </c>
       <c r="N22" s="15"/>
       <c r="P22" s="17"/>
-      <c r="Q22" s="200"/>
+      <c r="Q22" s="197"/>
       <c r="R22" s="28" t="s">
         <v>82</v>
       </c>
@@ -6841,7 +6766,7 @@
     </row>
     <row r="23" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
-      <c r="B23" s="199"/>
+      <c r="B23" s="196"/>
       <c r="C23" s="44" t="s">
         <v>83</v>
       </c>
@@ -6877,7 +6802,7 @@
       </c>
       <c r="N23" s="15"/>
       <c r="P23" s="17"/>
-      <c r="Q23" s="199"/>
+      <c r="Q23" s="196"/>
       <c r="R23" s="44" t="s">
         <v>83</v>
       </c>
@@ -6915,7 +6840,7 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24" s="17"/>
-      <c r="B24" s="198" t="s">
+      <c r="B24" s="195" t="s">
         <v>84</v>
       </c>
       <c r="C24" s="39" t="s">
@@ -6953,7 +6878,7 @@
       </c>
       <c r="N24" s="15"/>
       <c r="P24" s="17"/>
-      <c r="Q24" s="198" t="s">
+      <c r="Q24" s="195" t="s">
         <v>84</v>
       </c>
       <c r="R24" s="39" t="s">
@@ -6993,7 +6918,7 @@
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25" s="17"/>
-      <c r="B25" s="200"/>
+      <c r="B25" s="197"/>
       <c r="C25" s="28" t="s">
         <v>86</v>
       </c>
@@ -7029,7 +6954,7 @@
       </c>
       <c r="N25" s="15"/>
       <c r="P25" s="17"/>
-      <c r="Q25" s="200"/>
+      <c r="Q25" s="197"/>
       <c r="R25" s="28" t="s">
         <v>86</v>
       </c>
@@ -7067,7 +6992,7 @@
     </row>
     <row r="26" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
-      <c r="B26" s="199"/>
+      <c r="B26" s="196"/>
       <c r="C26" s="44" t="s">
         <v>87</v>
       </c>
@@ -7103,7 +7028,7 @@
       </c>
       <c r="N26" s="15"/>
       <c r="P26" s="17"/>
-      <c r="Q26" s="199"/>
+      <c r="Q26" s="196"/>
       <c r="R26" s="44" t="s">
         <v>87</v>
       </c>
@@ -7177,7 +7102,7 @@
       </c>
       <c r="N27" s="15"/>
       <c r="P27" s="17"/>
-      <c r="Q27" s="201" t="s">
+      <c r="Q27" s="198" t="s">
         <v>89</v>
       </c>
       <c r="R27" s="39" t="s">
@@ -7255,7 +7180,7 @@
       </c>
       <c r="N28" s="15"/>
       <c r="P28" s="17"/>
-      <c r="Q28" s="202"/>
+      <c r="Q28" s="199"/>
       <c r="R28" s="28" t="s">
         <v>90</v>
       </c>
@@ -7329,7 +7254,7 @@
       </c>
       <c r="N29" s="15"/>
       <c r="P29" s="17"/>
-      <c r="Q29" s="203"/>
+      <c r="Q29" s="200"/>
       <c r="R29" s="44" t="s">
         <v>91</v>
       </c>
@@ -7367,7 +7292,7 @@
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30" s="17"/>
-      <c r="B30" s="188" t="s">
+      <c r="B30" s="185" t="s">
         <v>92</v>
       </c>
       <c r="C30" s="39" t="s">
@@ -7405,7 +7330,7 @@
       </c>
       <c r="N30" s="15"/>
       <c r="P30" s="17"/>
-      <c r="Q30" s="188" t="s">
+      <c r="Q30" s="185" t="s">
         <v>92</v>
       </c>
       <c r="R30" s="39" t="s">
@@ -7445,7 +7370,7 @@
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31" s="17"/>
-      <c r="B31" s="189"/>
+      <c r="B31" s="186"/>
       <c r="C31" s="28" t="s">
         <v>94</v>
       </c>
@@ -7481,7 +7406,7 @@
       </c>
       <c r="N31" s="50"/>
       <c r="P31" s="17"/>
-      <c r="Q31" s="189"/>
+      <c r="Q31" s="186"/>
       <c r="R31" s="28" t="s">
         <v>94</v>
       </c>
@@ -7519,7 +7444,7 @@
     </row>
     <row r="32" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17"/>
-      <c r="B32" s="190"/>
+      <c r="B32" s="187"/>
       <c r="C32" s="44" t="s">
         <v>95</v>
       </c>
@@ -7555,7 +7480,7 @@
       </c>
       <c r="N32" s="15"/>
       <c r="P32" s="17"/>
-      <c r="Q32" s="190"/>
+      <c r="Q32" s="187"/>
       <c r="R32" s="44" t="s">
         <v>95</v>
       </c>
@@ -7593,10 +7518,10 @@
     </row>
     <row r="33" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
-      <c r="B33" s="182" t="s">
+      <c r="B33" s="179" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="183"/>
+      <c r="C33" s="180"/>
       <c r="D33" s="51">
         <v>7</v>
       </c>
@@ -7629,10 +7554,10 @@
       </c>
       <c r="N33" s="15"/>
       <c r="P33" s="17"/>
-      <c r="Q33" s="182" t="s">
+      <c r="Q33" s="179" t="s">
         <v>96</v>
       </c>
-      <c r="R33" s="183"/>
+      <c r="R33" s="180"/>
       <c r="S33" s="51">
         <v>0</v>
       </c>
@@ -7663,10 +7588,10 @@
     </row>
     <row r="34" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
-      <c r="B34" s="182" t="s">
+      <c r="B34" s="179" t="s">
         <v>97</v>
       </c>
-      <c r="C34" s="182"/>
+      <c r="C34" s="179"/>
       <c r="D34" s="52">
         <v>1.54</v>
       </c>
@@ -7701,10 +7626,10 @@
         <v>65</v>
       </c>
       <c r="P34" s="17"/>
-      <c r="Q34" s="182" t="s">
+      <c r="Q34" s="179" t="s">
         <v>97</v>
       </c>
-      <c r="R34" s="182"/>
+      <c r="R34" s="179"/>
       <c r="S34" s="52">
         <v>0</v>
       </c>
@@ -7737,69 +7662,69 @@
     </row>
     <row r="35" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
-      <c r="B35" s="182" t="s">
+      <c r="B35" s="179" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="183"/>
+      <c r="C35" s="180"/>
       <c r="D35" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="L35" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="L35" s="1" t="s">
+      <c r="M35" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="N35" s="15"/>
       <c r="P35" s="17"/>
-      <c r="Q35" s="182" t="s">
+      <c r="Q35" s="179" t="s">
         <v>98</v>
       </c>
-      <c r="R35" s="183"/>
+      <c r="R35" s="180"/>
       <c r="S35" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T35" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="U35" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="V35" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="W35" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="X35" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="W35" s="1" t="s">
+      <c r="Y35" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="Z35" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="X35" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="Y35" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="Z35" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="AA35" s="146"/>
       <c r="AB35" s="146"/>
@@ -7807,10 +7732,10 @@
     </row>
     <row r="36" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17"/>
-      <c r="B36" s="182" t="s">
+      <c r="B36" s="179" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="182"/>
+      <c r="C36" s="179"/>
       <c r="D36" s="33" t="s">
         <v>65</v>
       </c>
@@ -7825,12 +7750,12 @@
       <c r="M36" s="19"/>
       <c r="N36" s="15"/>
       <c r="P36" s="17"/>
-      <c r="Q36" s="182" t="s">
+      <c r="Q36" s="179" t="s">
         <v>99</v>
       </c>
-      <c r="R36" s="182"/>
+      <c r="R36" s="179"/>
       <c r="S36" s="161" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="T36" s="19"/>
       <c r="U36" s="19"/>
@@ -7954,34 +7879,34 @@
       </c>
       <c r="C39" s="55"/>
       <c r="D39" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="I39" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="J39" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N39" s="15"/>
       <c r="P39" s="54"/>
@@ -7990,28 +7915,28 @@
       </c>
       <c r="R39" s="55"/>
       <c r="S39" s="162" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T39" s="162" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="U39" s="162" t="s">
+        <v>181</v>
+      </c>
+      <c r="V39" s="162" t="s">
         <v>182</v>
       </c>
-      <c r="V39" s="162" t="s">
+      <c r="W39" s="162" t="s">
+        <v>181</v>
+      </c>
+      <c r="X39" s="162" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y39" s="162" t="s">
         <v>183</v>
       </c>
-      <c r="W39" s="162" t="s">
+      <c r="Z39" s="162" t="s">
         <v>182</v>
-      </c>
-      <c r="X39" s="162" t="s">
-        <v>181</v>
-      </c>
-      <c r="Y39" s="162" t="s">
-        <v>184</v>
-      </c>
-      <c r="Z39" s="162" t="s">
-        <v>183</v>
       </c>
       <c r="AA39" s="163"/>
       <c r="AB39" s="163"/>
@@ -8049,10 +7974,10 @@
     </row>
     <row r="41" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="56"/>
-      <c r="B41" s="184" t="s">
+      <c r="B41" s="181" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="185"/>
+      <c r="C41" s="182"/>
       <c r="D41" s="58" t="s">
         <v>102</v>
       </c>
@@ -8071,10 +7996,10 @@
       <c r="M41" s="10"/>
       <c r="N41" s="12"/>
       <c r="P41" s="56"/>
-      <c r="Q41" s="184" t="s">
+      <c r="Q41" s="181" t="s">
         <v>101</v>
       </c>
-      <c r="R41" s="185"/>
+      <c r="R41" s="182"/>
       <c r="S41" s="58" t="s">
         <v>102</v>
       </c>
@@ -8087,7 +8012,7 @@
       </c>
       <c r="Y41" s="10"/>
       <c r="Z41" s="164" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AA41" s="10"/>
       <c r="AB41" s="10"/>
@@ -8095,10 +8020,10 @@
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A42" s="56"/>
-      <c r="B42" s="186" t="s">
+      <c r="B42" s="183" t="s">
         <v>105</v>
       </c>
-      <c r="C42" s="187"/>
+      <c r="C42" s="184"/>
       <c r="D42" s="59"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
@@ -8111,10 +8036,10 @@
       <c r="M42" s="9"/>
       <c r="N42" s="12"/>
       <c r="P42" s="56"/>
-      <c r="Q42" s="186" t="s">
+      <c r="Q42" s="183" t="s">
         <v>105</v>
       </c>
-      <c r="R42" s="187"/>
+      <c r="R42" s="184"/>
       <c r="S42" s="59"/>
       <c r="T42" s="10"/>
       <c r="U42" s="10"/>
@@ -8129,10 +8054,10 @@
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A43" s="56"/>
-      <c r="B43" s="178" t="s">
+      <c r="B43" s="175" t="s">
         <v>106</v>
       </c>
-      <c r="C43" s="179"/>
+      <c r="C43" s="176"/>
       <c r="D43" s="60">
         <v>1</v>
       </c>
@@ -8147,10 +8072,10 @@
       <c r="M43" s="9"/>
       <c r="N43" s="12"/>
       <c r="P43" s="56"/>
-      <c r="Q43" s="178" t="s">
+      <c r="Q43" s="175" t="s">
         <v>106</v>
       </c>
-      <c r="R43" s="179"/>
+      <c r="R43" s="176"/>
       <c r="S43" s="60">
         <v>1</v>
       </c>
@@ -8167,10 +8092,10 @@
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A44" s="56"/>
-      <c r="B44" s="178" t="s">
+      <c r="B44" s="175" t="s">
         <v>107</v>
       </c>
-      <c r="C44" s="179"/>
+      <c r="C44" s="176"/>
       <c r="D44" s="61">
         <v>2</v>
       </c>
@@ -8185,10 +8110,10 @@
       <c r="M44" s="9"/>
       <c r="N44" s="12"/>
       <c r="P44" s="56"/>
-      <c r="Q44" s="178" t="s">
+      <c r="Q44" s="175" t="s">
         <v>107</v>
       </c>
-      <c r="R44" s="179"/>
+      <c r="R44" s="176"/>
       <c r="S44" s="61">
         <v>2</v>
       </c>
@@ -8205,10 +8130,10 @@
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45" s="56"/>
-      <c r="B45" s="178" t="s">
+      <c r="B45" s="175" t="s">
         <v>108</v>
       </c>
-      <c r="C45" s="179"/>
+      <c r="C45" s="176"/>
       <c r="D45" s="62">
         <v>3</v>
       </c>
@@ -8223,10 +8148,10 @@
       <c r="M45" s="9"/>
       <c r="N45" s="63"/>
       <c r="P45" s="56"/>
-      <c r="Q45" s="178" t="s">
+      <c r="Q45" s="175" t="s">
         <v>108</v>
       </c>
-      <c r="R45" s="179"/>
+      <c r="R45" s="176"/>
       <c r="S45" s="62">
         <v>3</v>
       </c>
@@ -8243,10 +8168,10 @@
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A46" s="56"/>
-      <c r="B46" s="180" t="s">
+      <c r="B46" s="177" t="s">
         <v>109</v>
       </c>
-      <c r="C46" s="181"/>
+      <c r="C46" s="178"/>
       <c r="D46" s="64">
         <v>4</v>
       </c>
@@ -8261,10 +8186,10 @@
       <c r="M46" s="9"/>
       <c r="N46" s="63"/>
       <c r="P46" s="56"/>
-      <c r="Q46" s="180" t="s">
+      <c r="Q46" s="177" t="s">
         <v>109</v>
       </c>
-      <c r="R46" s="181"/>
+      <c r="R46" s="178"/>
       <c r="S46" s="64">
         <v>4</v>
       </c>
@@ -9288,19 +9213,19 @@
       <c r="C1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="206" t="s">
+      <c r="D1" s="203" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="206"/>
-      <c r="F1" s="206"/>
+      <c r="E1" s="203"/>
+      <c r="F1" s="203"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="241" t="s">
+      <c r="I1" s="238" t="s">
         <v>112</v>
       </c>
-      <c r="J1" s="241"/>
+      <c r="J1" s="238"/>
       <c r="K1" s="76"/>
       <c r="L1" s="104"/>
       <c r="N1" s="75" t="s">
@@ -9310,19 +9235,19 @@
       <c r="P1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="206" t="s">
+      <c r="Q1" s="203" t="s">
         <v>110</v>
       </c>
-      <c r="R1" s="206"/>
-      <c r="S1" s="206"/>
+      <c r="R1" s="203"/>
+      <c r="S1" s="203"/>
       <c r="T1" s="5"/>
       <c r="U1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="V1" s="241" t="s">
+      <c r="V1" s="238" t="s">
         <v>112</v>
       </c>
-      <c r="W1" s="241"/>
+      <c r="W1" s="238"/>
       <c r="X1" s="76"/>
       <c r="Y1" s="104"/>
     </row>
@@ -9334,11 +9259,11 @@
       <c r="C2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="242" t="s">
+      <c r="D2" s="239" t="s">
         <v>111</v>
       </c>
-      <c r="E2" s="242"/>
-      <c r="F2" s="242"/>
+      <c r="E2" s="239"/>
+      <c r="F2" s="239"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10" t="s">
         <v>116</v>
@@ -9356,11 +9281,11 @@
       <c r="P2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" s="242" t="s">
+      <c r="Q2" s="239" t="s">
         <v>111</v>
       </c>
-      <c r="R2" s="242"/>
-      <c r="S2" s="242"/>
+      <c r="R2" s="239"/>
+      <c r="S2" s="239"/>
       <c r="T2" s="10"/>
       <c r="U2" s="10" t="s">
         <v>145</v>
@@ -9373,42 +9298,42 @@
       <c r="Y2" s="105"/>
     </row>
     <row r="3" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="243" t="s">
+      <c r="A3" s="240" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="244"/>
-      <c r="C3" s="247" t="s">
+      <c r="B3" s="241"/>
+      <c r="C3" s="244" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="247"/>
-      <c r="E3" s="247"/>
-      <c r="F3" s="247"/>
-      <c r="G3" s="247"/>
-      <c r="H3" s="247"/>
-      <c r="I3" s="247"/>
-      <c r="J3" s="247"/>
-      <c r="K3" s="247"/>
-      <c r="L3" s="248"/>
-      <c r="N3" s="243" t="s">
+      <c r="D3" s="244"/>
+      <c r="E3" s="244"/>
+      <c r="F3" s="244"/>
+      <c r="G3" s="244"/>
+      <c r="H3" s="244"/>
+      <c r="I3" s="244"/>
+      <c r="J3" s="244"/>
+      <c r="K3" s="244"/>
+      <c r="L3" s="245"/>
+      <c r="N3" s="240" t="s">
         <v>117</v>
       </c>
-      <c r="O3" s="244"/>
-      <c r="P3" s="247" t="s">
+      <c r="O3" s="241"/>
+      <c r="P3" s="244" t="s">
         <v>118</v>
       </c>
-      <c r="Q3" s="247"/>
-      <c r="R3" s="247"/>
-      <c r="S3" s="247"/>
-      <c r="T3" s="247"/>
-      <c r="U3" s="247"/>
-      <c r="V3" s="247"/>
-      <c r="W3" s="247"/>
-      <c r="X3" s="247"/>
-      <c r="Y3" s="248"/>
+      <c r="Q3" s="244"/>
+      <c r="R3" s="244"/>
+      <c r="S3" s="244"/>
+      <c r="T3" s="244"/>
+      <c r="U3" s="244"/>
+      <c r="V3" s="244"/>
+      <c r="W3" s="244"/>
+      <c r="X3" s="244"/>
+      <c r="Y3" s="245"/>
     </row>
     <row r="4" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="243"/>
-      <c r="B4" s="244"/>
+      <c r="A4" s="240"/>
+      <c r="B4" s="241"/>
       <c r="C4" s="79">
         <v>1</v>
       </c>
@@ -9439,8 +9364,8 @@
       <c r="L4" s="106">
         <v>10</v>
       </c>
-      <c r="N4" s="245"/>
-      <c r="O4" s="246"/>
+      <c r="N4" s="242"/>
+      <c r="O4" s="243"/>
       <c r="P4" s="79">
         <v>11</v>
       </c>
@@ -9473,10 +9398,10 @@
       </c>
     </row>
     <row r="5" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="232" t="s">
+      <c r="A5" s="229" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="233"/>
+      <c r="B5" s="230"/>
       <c r="C5" s="82" t="s">
         <v>5</v>
       </c>
@@ -9507,10 +9432,10 @@
       <c r="L5" s="139" t="s">
         <v>26</v>
       </c>
-      <c r="N5" s="249" t="s">
+      <c r="N5" s="246" t="s">
         <v>119</v>
       </c>
-      <c r="O5" s="250"/>
+      <c r="O5" s="247"/>
       <c r="P5" s="107" t="s">
         <v>28</v>
       </c>
@@ -9539,10 +9464,10 @@
       <c r="Y5" s="110"/>
     </row>
     <row r="6" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="232" t="s">
+      <c r="A6" s="229" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="233"/>
+      <c r="B6" s="230"/>
       <c r="C6" s="85" t="s">
         <v>6</v>
       </c>
@@ -9573,10 +9498,10 @@
       <c r="L6" s="140" t="s">
         <v>27</v>
       </c>
-      <c r="N6" s="249" t="s">
+      <c r="N6" s="246" t="s">
         <v>120</v>
       </c>
-      <c r="O6" s="250"/>
+      <c r="O6" s="247"/>
       <c r="P6" s="89" t="s">
         <v>29</v>
       </c>
@@ -9605,10 +9530,10 @@
       <c r="Y6" s="112"/>
     </row>
     <row r="7" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="232" t="s">
+      <c r="A7" s="229" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="233"/>
+      <c r="B7" s="230"/>
       <c r="C7" s="85">
         <v>105</v>
       </c>
@@ -9639,10 +9564,10 @@
       <c r="L7" s="135">
         <v>121</v>
       </c>
-      <c r="N7" s="251" t="s">
+      <c r="N7" s="248" t="s">
         <v>121</v>
       </c>
-      <c r="O7" s="252"/>
+      <c r="O7" s="249"/>
       <c r="P7" s="89">
         <v>105</v>
       </c>
@@ -9671,10 +9596,10 @@
       <c r="Y7" s="115"/>
     </row>
     <row r="8" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="232" t="s">
+      <c r="A8" s="229" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="233"/>
+      <c r="B8" s="230"/>
       <c r="C8" s="88">
         <v>1</v>
       </c>
@@ -9705,10 +9630,10 @@
       <c r="L8" s="142">
         <v>2</v>
       </c>
-      <c r="N8" s="230" t="s">
+      <c r="N8" s="227" t="s">
         <v>122</v>
       </c>
-      <c r="O8" s="231"/>
+      <c r="O8" s="228"/>
       <c r="P8" s="88">
         <v>1</v>
       </c>
@@ -9741,10 +9666,10 @@
       </c>
     </row>
     <row r="9" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="232" t="s">
+      <c r="A9" s="229" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="233"/>
+      <c r="B9" s="230"/>
       <c r="C9" s="90" t="s">
         <v>113</v>
       </c>
@@ -9775,10 +9700,10 @@
       <c r="L9" s="143" t="s">
         <v>113</v>
       </c>
-      <c r="N9" s="232" t="s">
+      <c r="N9" s="229" t="s">
         <v>123</v>
       </c>
-      <c r="O9" s="233"/>
+      <c r="O9" s="230"/>
       <c r="P9" s="90" t="s">
         <v>113</v>
       </c>
@@ -9811,37 +9736,37 @@
       </c>
     </row>
     <row r="10" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="257"/>
-      <c r="B10" s="258"/>
-      <c r="C10" s="234" t="s">
+      <c r="A10" s="254"/>
+      <c r="B10" s="255"/>
+      <c r="C10" s="231" t="s">
         <v>124</v>
       </c>
-      <c r="D10" s="234"/>
-      <c r="E10" s="234"/>
-      <c r="F10" s="234"/>
-      <c r="G10" s="234"/>
-      <c r="H10" s="234"/>
-      <c r="I10" s="234"/>
-      <c r="J10" s="234"/>
-      <c r="K10" s="234"/>
-      <c r="L10" s="235"/>
+      <c r="D10" s="231"/>
+      <c r="E10" s="231"/>
+      <c r="F10" s="231"/>
+      <c r="G10" s="231"/>
+      <c r="H10" s="231"/>
+      <c r="I10" s="231"/>
+      <c r="J10" s="231"/>
+      <c r="K10" s="231"/>
+      <c r="L10" s="232"/>
       <c r="N10" s="144"/>
       <c r="O10" s="145"/>
-      <c r="P10" s="234" t="s">
+      <c r="P10" s="231" t="s">
         <v>124</v>
       </c>
-      <c r="Q10" s="234"/>
-      <c r="R10" s="234"/>
-      <c r="S10" s="234"/>
-      <c r="T10" s="234"/>
-      <c r="U10" s="234"/>
-      <c r="V10" s="234"/>
-      <c r="W10" s="234"/>
-      <c r="X10" s="234"/>
-      <c r="Y10" s="235"/>
+      <c r="Q10" s="231"/>
+      <c r="R10" s="231"/>
+      <c r="S10" s="231"/>
+      <c r="T10" s="231"/>
+      <c r="U10" s="231"/>
+      <c r="V10" s="231"/>
+      <c r="W10" s="231"/>
+      <c r="X10" s="231"/>
+      <c r="Y10" s="232"/>
     </row>
     <row r="11" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="236" t="s">
+      <c r="A11" s="233" t="s">
         <v>125</v>
       </c>
       <c r="B11" s="81" t="s">
@@ -9877,7 +9802,7 @@
       <c r="L11" s="139" t="s">
         <v>113</v>
       </c>
-      <c r="N11" s="236" t="s">
+      <c r="N11" s="233" t="s">
         <v>125</v>
       </c>
       <c r="O11" s="81" t="s">
@@ -9915,7 +9840,7 @@
       </c>
     </row>
     <row r="12" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="237"/>
+      <c r="A12" s="234"/>
       <c r="B12" s="81" t="s">
         <v>127</v>
       </c>
@@ -9949,7 +9874,7 @@
       <c r="L12" s="140" t="s">
         <v>113</v>
       </c>
-      <c r="N12" s="237"/>
+      <c r="N12" s="234"/>
       <c r="O12" s="81" t="s">
         <v>127</v>
       </c>
@@ -9985,7 +9910,7 @@
       </c>
     </row>
     <row r="13" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="237"/>
+      <c r="A13" s="234"/>
       <c r="B13" s="81" t="s">
         <v>128</v>
       </c>
@@ -10019,7 +9944,7 @@
       <c r="L13" s="140" t="s">
         <v>113</v>
       </c>
-      <c r="N13" s="237"/>
+      <c r="N13" s="234"/>
       <c r="O13" s="81" t="s">
         <v>128</v>
       </c>
@@ -10055,7 +9980,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="237"/>
+      <c r="A14" s="234"/>
       <c r="B14" s="81" t="s">
         <v>129</v>
       </c>
@@ -10089,7 +10014,7 @@
       <c r="L14" s="140" t="s">
         <v>113</v>
       </c>
-      <c r="N14" s="237"/>
+      <c r="N14" s="234"/>
       <c r="O14" s="81" t="s">
         <v>129</v>
       </c>
@@ -10125,7 +10050,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="238"/>
+      <c r="A15" s="235"/>
       <c r="B15" s="81" t="s">
         <v>130</v>
       </c>
@@ -10159,7 +10084,7 @@
       <c r="L15" s="140" t="s">
         <v>113</v>
       </c>
-      <c r="N15" s="238"/>
+      <c r="N15" s="235"/>
       <c r="O15" s="81" t="s">
         <v>130</v>
       </c>
@@ -10195,10 +10120,10 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="232" t="s">
+      <c r="A16" s="229" t="s">
         <v>131</v>
       </c>
-      <c r="B16" s="233"/>
+      <c r="B16" s="230"/>
       <c r="C16" s="92" t="s">
         <v>113</v>
       </c>
@@ -10229,10 +10154,10 @@
       <c r="L16" s="140" t="s">
         <v>113</v>
       </c>
-      <c r="N16" s="232" t="s">
+      <c r="N16" s="229" t="s">
         <v>131</v>
       </c>
-      <c r="O16" s="233"/>
+      <c r="O16" s="230"/>
       <c r="P16" s="92" t="s">
         <v>113</v>
       </c>
@@ -10265,10 +10190,10 @@
       </c>
     </row>
     <row r="17" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="232" t="s">
+      <c r="A17" s="229" t="s">
         <v>132</v>
       </c>
-      <c r="B17" s="233"/>
+      <c r="B17" s="230"/>
       <c r="C17" s="93" t="s">
         <v>113</v>
       </c>
@@ -10299,10 +10224,10 @@
       <c r="L17" s="141" t="s">
         <v>146</v>
       </c>
-      <c r="N17" s="232" t="s">
+      <c r="N17" s="229" t="s">
         <v>132</v>
       </c>
-      <c r="O17" s="233"/>
+      <c r="O17" s="230"/>
       <c r="P17" s="93" t="s">
         <v>113</v>
       </c>
@@ -10335,40 +10260,40 @@
       </c>
     </row>
     <row r="18" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="255"/>
-      <c r="B18" s="256"/>
-      <c r="C18" s="226" t="s">
+      <c r="A18" s="252"/>
+      <c r="B18" s="253"/>
+      <c r="C18" s="223" t="s">
         <v>133</v>
       </c>
-      <c r="D18" s="226"/>
-      <c r="E18" s="226"/>
-      <c r="F18" s="226"/>
-      <c r="G18" s="226"/>
-      <c r="H18" s="226"/>
-      <c r="I18" s="226"/>
-      <c r="J18" s="226"/>
-      <c r="K18" s="226"/>
-      <c r="L18" s="227"/>
+      <c r="D18" s="223"/>
+      <c r="E18" s="223"/>
+      <c r="F18" s="223"/>
+      <c r="G18" s="223"/>
+      <c r="H18" s="223"/>
+      <c r="I18" s="223"/>
+      <c r="J18" s="223"/>
+      <c r="K18" s="223"/>
+      <c r="L18" s="224"/>
       <c r="N18" s="56"/>
       <c r="O18" s="10"/>
-      <c r="P18" s="226" t="s">
+      <c r="P18" s="223" t="s">
         <v>133</v>
       </c>
-      <c r="Q18" s="226"/>
-      <c r="R18" s="226"/>
-      <c r="S18" s="226"/>
-      <c r="T18" s="226"/>
-      <c r="U18" s="226"/>
-      <c r="V18" s="226"/>
-      <c r="W18" s="226"/>
-      <c r="X18" s="226"/>
-      <c r="Y18" s="227"/>
+      <c r="Q18" s="223"/>
+      <c r="R18" s="223"/>
+      <c r="S18" s="223"/>
+      <c r="T18" s="223"/>
+      <c r="U18" s="223"/>
+      <c r="V18" s="223"/>
+      <c r="W18" s="223"/>
+      <c r="X18" s="223"/>
+      <c r="Y18" s="224"/>
     </row>
     <row r="19" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="220" t="s">
+      <c r="A19" s="217" t="s">
         <v>134</v>
       </c>
-      <c r="B19" s="221"/>
+      <c r="B19" s="218"/>
       <c r="C19" s="82" t="s">
         <v>113</v>
       </c>
@@ -10399,10 +10324,10 @@
       <c r="L19" s="134" t="s">
         <v>113</v>
       </c>
-      <c r="N19" s="220" t="s">
+      <c r="N19" s="217" t="s">
         <v>134</v>
       </c>
-      <c r="O19" s="221"/>
+      <c r="O19" s="218"/>
       <c r="P19" s="82" t="s">
         <v>113</v>
       </c>
@@ -10435,10 +10360,10 @@
       </c>
     </row>
     <row r="20" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="220" t="s">
+      <c r="A20" s="217" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="221"/>
+      <c r="B20" s="218"/>
       <c r="C20" s="92" t="s">
         <v>113</v>
       </c>
@@ -10469,10 +10394,10 @@
       <c r="L20" s="135" t="s">
         <v>113</v>
       </c>
-      <c r="N20" s="220" t="s">
+      <c r="N20" s="217" t="s">
         <v>135</v>
       </c>
-      <c r="O20" s="221"/>
+      <c r="O20" s="218"/>
       <c r="P20" s="92" t="s">
         <v>113</v>
       </c>
@@ -10505,10 +10430,10 @@
       </c>
     </row>
     <row r="21" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="220" t="s">
+      <c r="A21" s="217" t="s">
         <v>136</v>
       </c>
-      <c r="B21" s="221"/>
+      <c r="B21" s="218"/>
       <c r="C21" s="92" t="s">
         <v>113</v>
       </c>
@@ -10539,10 +10464,10 @@
       <c r="L21" s="135" t="s">
         <v>113</v>
       </c>
-      <c r="N21" s="220" t="s">
+      <c r="N21" s="217" t="s">
         <v>136</v>
       </c>
-      <c r="O21" s="221"/>
+      <c r="O21" s="218"/>
       <c r="P21" s="92" t="s">
         <v>113</v>
       </c>
@@ -10575,10 +10500,10 @@
       </c>
     </row>
     <row r="22" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="220" t="s">
+      <c r="A22" s="217" t="s">
         <v>137</v>
       </c>
-      <c r="B22" s="221"/>
+      <c r="B22" s="218"/>
       <c r="C22" s="92">
         <v>20</v>
       </c>
@@ -10609,10 +10534,10 @@
       <c r="L22" s="135" t="s">
         <v>113</v>
       </c>
-      <c r="N22" s="220" t="s">
+      <c r="N22" s="217" t="s">
         <v>137</v>
       </c>
-      <c r="O22" s="221"/>
+      <c r="O22" s="218"/>
       <c r="P22" s="92" t="s">
         <v>148</v>
       </c>
@@ -10645,10 +10570,10 @@
       </c>
     </row>
     <row r="23" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="176" t="s">
+      <c r="A23" s="173" t="s">
         <v>138</v>
       </c>
-      <c r="B23" s="177" t="s">
+      <c r="B23" s="174" t="s">
         <v>139</v>
       </c>
       <c r="C23" s="98"/>
@@ -10679,10 +10604,10 @@
       <c r="Y23" s="129"/>
     </row>
     <row r="24" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="228" t="s">
+      <c r="A24" s="225" t="s">
         <v>140</v>
       </c>
-      <c r="B24" s="229"/>
+      <c r="B24" s="226"/>
       <c r="C24" s="92" t="s">
         <v>113</v>
       </c>
@@ -10713,10 +10638,10 @@
       <c r="L24" s="135" t="s">
         <v>113</v>
       </c>
-      <c r="N24" s="228" t="s">
+      <c r="N24" s="225" t="s">
         <v>140</v>
       </c>
-      <c r="O24" s="229"/>
+      <c r="O24" s="226"/>
       <c r="P24" s="92" t="s">
         <v>113</v>
       </c>
@@ -10749,10 +10674,10 @@
       </c>
     </row>
     <row r="25" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="222" t="s">
+      <c r="A25" s="219" t="s">
         <v>141</v>
       </c>
-      <c r="B25" s="223"/>
+      <c r="B25" s="220"/>
       <c r="C25" s="92" t="s">
         <v>113</v>
       </c>
@@ -10783,10 +10708,10 @@
       <c r="L25" s="135" t="s">
         <v>113</v>
       </c>
-      <c r="N25" s="220" t="s">
+      <c r="N25" s="217" t="s">
         <v>141</v>
       </c>
-      <c r="O25" s="221"/>
+      <c r="O25" s="218"/>
       <c r="P25" s="92" t="s">
         <v>113</v>
       </c>
@@ -10819,10 +10744,10 @@
       </c>
     </row>
     <row r="26" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="253" t="s">
+      <c r="A26" s="250" t="s">
         <v>142</v>
       </c>
-      <c r="B26" s="254"/>
+      <c r="B26" s="251"/>
       <c r="C26" s="100" t="s">
         <v>113</v>
       </c>
@@ -10853,10 +10778,10 @@
       <c r="L26" s="137" t="s">
         <v>113</v>
       </c>
-      <c r="N26" s="222" t="s">
+      <c r="N26" s="219" t="s">
         <v>142</v>
       </c>
-      <c r="O26" s="223"/>
+      <c r="O26" s="220"/>
       <c r="P26" s="100" t="s">
         <v>113</v>
       </c>
@@ -10889,10 +10814,10 @@
       </c>
     </row>
     <row r="27" spans="1:25" ht="83.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="224" t="s">
+      <c r="A27" s="221" t="s">
         <v>143</v>
       </c>
-      <c r="B27" s="239"/>
+      <c r="B27" s="236"/>
       <c r="C27" s="102" t="s">
         <v>150</v>
       </c>
@@ -10923,10 +10848,10 @@
       <c r="L27" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="N27" s="224" t="s">
+      <c r="N27" s="221" t="s">
         <v>143</v>
       </c>
-      <c r="O27" s="225"/>
+      <c r="O27" s="222"/>
       <c r="P27" s="103" t="s">
         <v>158</v>
       </c>
@@ -10959,8 +10884,8 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A28" s="240"/>
-      <c r="B28" s="240"/>
+      <c r="A28" s="237"/>
+      <c r="B28" s="237"/>
     </row>
   </sheetData>
   <mergeCells count="49">
@@ -11034,6 +10959,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="d699723c-6030-48dd-835b-9dac49e7a8e6" xsi:nil="true"/>
@@ -11044,7 +10978,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101006D53F4C8D732D844AE7D882D8C27E66C" ma:contentTypeVersion="18" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="70bbe916ee44c898308fc52b233fdc6f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2d274541-22b4-4212-af6c-71d9850896b1" xmlns:ns3="d699723c-6030-48dd-835b-9dac49e7a8e6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d0e6162704bbcf8652c04252123e2ebc" ns2:_="" ns3:_="">
     <xsd:import namespace="2d274541-22b4-4212-af6c-71d9850896b1"/>
@@ -11299,16 +11233,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41795C53-3181-4C52-8680-4752CA0088F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06DBE990-EB98-4F68-B739-71C82D62973A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11319,7 +11252,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAE067A7-9A28-427F-B4BA-DF647AB143B9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11336,12 +11269,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41795C53-3181-4C52-8680-4752CA0088F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated README and DbSeeder.cs. Changed ConnectionStrings to use LocalConnection. Uploaded updated Rapporter.xlsx template.
</commit_message>
<xml_diff>
--- a/SeaEco.Server/wwwroot/reports/Rapporter.xlsx
+++ b/SeaEco.Server/wwwroot/reports/Rapporter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tetianaverkhalantseva/RiderProjects/SeaEco/SeaEco.Server/wwwroot/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3542D429-208D-3747-B16C-F9A2F53D29BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3868E3A-7B76-C042-8CEC-40227818CF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16660" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21860" windowHeight="16620" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="5" r:id="rId1"/>
@@ -19,8 +19,7 @@
     <sheet name="B1 Skjema" sheetId="3" r:id="rId4"/>
     <sheet name="B2 Skjema" sheetId="4" r:id="rId5"/>
     <sheet name="Bilder" sheetId="7" r:id="rId6"/>
-    <sheet name="pHEh" sheetId="2" r:id="rId7"/>
-    <sheet name="PhEh-Plot" sheetId="8" r:id="rId8"/>
+    <sheet name="PhEh-Plot" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,10 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="139">
-  <si>
-    <t>St.nr.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="135">
   <si>
     <t>Nordlig</t>
   </si>
@@ -55,9 +51,6 @@
   </si>
   <si>
     <t>Dybde (m)</t>
-  </si>
-  <si>
-    <t>Ant. forsøk på prøvetaking</t>
   </si>
   <si>
     <t>Hard (H)/ 
@@ -91,9 +84,6 @@
     <t>Poeng</t>
   </si>
   <si>
-    <t xml:space="preserve">Prøvenr. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Indeks: </t>
   </si>
   <si>
@@ -104,9 +94,6 @@
   </si>
   <si>
     <t>Dyr</t>
-  </si>
-  <si>
-    <t>Ja=0, Nei=1</t>
   </si>
   <si>
     <t>II</t>
@@ -145,9 +132,6 @@
     </r>
   </si>
   <si>
-    <t>fra fig. D1</t>
-  </si>
-  <si>
     <t>se neste side</t>
   </si>
   <si>
@@ -163,12 +147,6 @@
     <t>Sediment ºC:</t>
   </si>
   <si>
-    <t xml:space="preserve">pH-sjø: </t>
-  </si>
-  <si>
-    <t>Eh sjø:</t>
-  </si>
-  <si>
     <t>Ref.elektrode:</t>
   </si>
   <si>
@@ -178,69 +156,21 @@
     <t>Gassbobler</t>
   </si>
   <si>
-    <t>Ja=4</t>
-  </si>
-  <si>
-    <t>Nei=0</t>
-  </si>
-  <si>
     <t>Farge</t>
   </si>
   <si>
-    <t>Lys grå=0</t>
-  </si>
-  <si>
-    <t>Brun/svart=2</t>
-  </si>
-  <si>
     <t>Lukt</t>
   </si>
   <si>
-    <t>Ingen=0</t>
-  </si>
-  <si>
-    <t>Noe=2</t>
-  </si>
-  <si>
-    <t>Sterk=4</t>
-  </si>
-  <si>
     <t>Konsistens</t>
   </si>
   <si>
-    <t>Fast=0</t>
-  </si>
-  <si>
-    <t>Myk=2</t>
-  </si>
-  <si>
-    <t>Løs=4</t>
-  </si>
-  <si>
-    <t>&lt;1/4 =0</t>
-  </si>
-  <si>
     <t>Grabbvolum</t>
   </si>
   <si>
-    <t>1/4-3/4=1</t>
-  </si>
-  <si>
-    <t>&gt;3/4=2</t>
-  </si>
-  <si>
     <t>Tykkelse på slamlag</t>
   </si>
   <si>
-    <t>0-2 cm=0</t>
-  </si>
-  <si>
-    <t>2-8 cm =1</t>
-  </si>
-  <si>
-    <t>&gt;8 cm=2</t>
-  </si>
-  <si>
     <t>SUM</t>
   </si>
   <si>
@@ -292,15 +222,9 @@
     <t>del 1 av 2</t>
   </si>
   <si>
-    <t>ID.:</t>
-  </si>
-  <si>
     <t>Informasjon fra prøvepunkt</t>
   </si>
   <si>
-    <t>Prøvepunkter</t>
-  </si>
-  <si>
     <t>Posisjon                   N</t>
   </si>
   <si>
@@ -346,27 +270,9 @@
     <t>Bunndyrsanalyse</t>
   </si>
   <si>
-    <t>Pigghuder (ant)</t>
-  </si>
-  <si>
-    <t>Krepsdyr (ant)</t>
-  </si>
-  <si>
-    <t>Skjell (ant)</t>
-  </si>
-  <si>
-    <t>Børstemark (ant)</t>
-  </si>
-  <si>
     <t>Andre dyr</t>
   </si>
   <si>
-    <t>tot. ant.</t>
-  </si>
-  <si>
-    <t>Beggiota</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fôr </t>
   </si>
   <si>
@@ -379,25 +285,7 @@
     <t>del 2 av 2</t>
   </si>
   <si>
-    <t>Lokalitetsnr.:</t>
-  </si>
-  <si>
     <t>Beskrivelse</t>
-  </si>
-  <si>
-    <t>Antall stasjoner</t>
-  </si>
-  <si>
-    <t>Total stasjoner</t>
-  </si>
-  <si>
-    <t>St. med dyr</t>
-  </si>
-  <si>
-    <t>St. med pH/Eh</t>
-  </si>
-  <si>
-    <t>Total grabbhugg</t>
   </si>
   <si>
     <t xml:space="preserve">Andel </t>
@@ -434,9 +322,6 @@
     <t>Antall hardbunn</t>
   </si>
   <si>
-    <t>Totalt antall stajsoner</t>
-  </si>
-  <si>
     <t>Hardbunnsstasjoner</t>
   </si>
   <si>
@@ -476,13 +361,125 @@
     <t>Analyser</t>
   </si>
   <si>
-    <t>St. nr.</t>
-  </si>
-  <si>
     <t>Usilt</t>
   </si>
   <si>
     <t>BILDER AV PRØVENE</t>
+  </si>
+  <si>
+    <t>Stasjoner totalt</t>
+  </si>
+  <si>
+    <t>Antall grabbhugg</t>
+  </si>
+  <si>
+    <t>Stasjoner med dyr</t>
+  </si>
+  <si>
+    <t>Stasjoner med pH/Eh</t>
+  </si>
+  <si>
+    <t>Antall</t>
+  </si>
+  <si>
+    <t>Antall stajsoner</t>
+  </si>
+  <si>
+    <t>Ja = 0, Nei = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pH sjø: </t>
+  </si>
+  <si>
+    <t>Eh sjø (mV):</t>
+  </si>
+  <si>
+    <t>Ja = 4</t>
+  </si>
+  <si>
+    <t>Nei = 0</t>
+  </si>
+  <si>
+    <t>Lys grå = 0</t>
+  </si>
+  <si>
+    <t>Brun/svart = 2</t>
+  </si>
+  <si>
+    <t>Ingen = 0</t>
+  </si>
+  <si>
+    <t>Noe = 2</t>
+  </si>
+  <si>
+    <t>Sterk = 4</t>
+  </si>
+  <si>
+    <t>Fast = 0</t>
+  </si>
+  <si>
+    <t>Myk = 2</t>
+  </si>
+  <si>
+    <t>Løs = 4</t>
+  </si>
+  <si>
+    <t>&lt;1/4 = 0</t>
+  </si>
+  <si>
+    <t>1/4-3/4 = 1</t>
+  </si>
+  <si>
+    <t>&gt;3/4 = 2</t>
+  </si>
+  <si>
+    <t>0-2 cm = 0</t>
+  </si>
+  <si>
+    <t>2-8 cm = 1</t>
+  </si>
+  <si>
+    <t>&gt;8 cm = 2</t>
+  </si>
+  <si>
+    <t>Tilstand gruppe III</t>
+  </si>
+  <si>
+    <t>Prøvenummer</t>
+  </si>
+  <si>
+    <t>fra fiigur D1</t>
+  </si>
+  <si>
+    <t>fra figur D1</t>
+  </si>
+  <si>
+    <t>Pigghuder (antall)</t>
+  </si>
+  <si>
+    <t>Krepsdyr (antall)</t>
+  </si>
+  <si>
+    <t>Skjell (antall)</t>
+  </si>
+  <si>
+    <t>Børstemark (antall)</t>
+  </si>
+  <si>
+    <t>totalt antall</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Beggiatoa </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial Nova Cond"/>
+        <family val="2"/>
+      </rPr>
+      <t>sp.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -492,7 +489,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="40" x14ac:knownFonts="1">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -667,11 +664,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial Nova Cond"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -755,6 +747,16 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial Nova Cond"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <name val="Arial Nova Cond"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -2444,14 +2446,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="84" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2467,34 +2469,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2519,10 +2521,10 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="52" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -2693,10 +2695,10 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2774,10 +2776,10 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2786,7 +2788,7 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4621,55 +4623,6 @@
         <a:xfrm>
           <a:off x="4913993" y="0"/>
           <a:ext cx="972910" cy="284842"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>473746</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>66125</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Bilde 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFD18BB9-A2EB-4F3F-8A63-09A44C481224}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="8285847" cy="6565537"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4947,10 +4900,10 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" customWidth="1"/>
@@ -4959,7 +4912,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="124" t="s">
-        <v>124</v>
+        <v>86</v>
       </c>
       <c r="B1" s="160"/>
       <c r="C1" s="130"/>
@@ -4971,7 +4924,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="131" t="s">
-        <v>125</v>
+        <v>87</v>
       </c>
       <c r="B2" s="195"/>
       <c r="C2" s="195"/>
@@ -4982,159 +4935,159 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="124" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="B4" s="125" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="126" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B5" s="127"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="126" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B6" s="127"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="126" t="s">
-        <v>123</v>
+        <v>85</v>
       </c>
       <c r="B7" s="127"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="126" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B8" s="127"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="126" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B9" s="127"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="124" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B11" s="125" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="128" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="B12" s="127"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="128" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="B13" s="127"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="128" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="B14" s="127"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="128" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="B15" s="127"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="128" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="B16" s="127"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="128" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="B17" s="127"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="128" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="B18" s="127"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="124" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="125" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="125" t="s">
-        <v>122</v>
-      </c>
       <c r="C20" s="125" t="s">
-        <v>121</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="128" t="s">
-        <v>117</v>
+        <v>80</v>
       </c>
       <c r="B21" s="127"/>
       <c r="C21" s="127"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="128" t="s">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="B22" s="127"/>
       <c r="C22" s="127"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="128" t="s">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="B23" s="127"/>
       <c r="C23" s="127"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="128" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="B24" s="127"/>
       <c r="C24" s="127"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="124" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="B26" s="125" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="C26" s="125" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="128" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="B27" s="127"/>
       <c r="C27" s="127"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="128" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
       <c r="B28" s="127"/>
       <c r="C28" s="127"/>
     </row>
     <row r="29" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="129" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="B29" s="127"/>
       <c r="C29" s="127"/>
@@ -5184,7 +5137,7 @@
     </row>
     <row r="3" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="200" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="B3" s="200"/>
       <c r="C3" s="200"/>
@@ -5207,12 +5160,12 @@
     <row r="5" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="175" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="B6" s="201"/>
       <c r="C6" s="201"/>
       <c r="D6" s="202" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="E6" s="202"/>
       <c r="F6" s="203"/>
@@ -5221,12 +5174,12 @@
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="175" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="B7" s="201"/>
       <c r="C7" s="201"/>
       <c r="D7" s="202" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="E7" s="202"/>
       <c r="F7" s="204"/>
@@ -5236,22 +5189,22 @@
     <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:8" ht="32.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="177" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="B9" s="178" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="C9" s="196" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="D9" s="197"/>
       <c r="E9" s="197"/>
       <c r="F9" s="198"/>
       <c r="G9" s="178" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="H9" s="179" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -6961,7 +6914,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6972,22 +6925,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -7159,11 +7112,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73EE1091-9F45-40A9-90F5-6AF0F1D8D5C5}">
   <dimension ref="A1:AC50"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="117" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+    <sheetView zoomScale="117" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="64" customWidth="1"/>
     <col min="2" max="2" width="11" style="64" customWidth="1"/>
@@ -7177,40 +7130,40 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="231" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="232"/>
       <c r="C1" s="232"/>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F1" s="233"/>
       <c r="G1" s="233"/>
       <c r="H1" s="233"/>
       <c r="I1" s="5"/>
       <c r="J1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K1" s="234"/>
       <c r="L1" s="234"/>
       <c r="M1" s="6"/>
       <c r="N1" s="7"/>
       <c r="P1" s="231" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q1" s="232"/>
       <c r="R1" s="232"/>
       <c r="S1" s="3"/>
       <c r="T1" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="U1" s="233"/>
       <c r="V1" s="233"/>
       <c r="W1" s="233"/>
       <c r="X1" s="5"/>
       <c r="Y1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Z1" s="234"/>
       <c r="AA1" s="234"/>
@@ -7219,40 +7172,40 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="245" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="246"/>
       <c r="C2" s="246"/>
       <c r="D2" s="8"/>
       <c r="E2" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F2" s="237"/>
       <c r="G2" s="237"/>
       <c r="H2" s="237"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K2" s="161"/>
       <c r="L2" s="9"/>
       <c r="M2" s="9"/>
       <c r="N2" s="10"/>
       <c r="P2" s="235" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="Q2" s="236"/>
       <c r="R2" s="236"/>
       <c r="S2" s="8"/>
       <c r="T2" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U2" s="237"/>
       <c r="V2" s="237"/>
       <c r="W2" s="237"/>
       <c r="X2" s="9"/>
       <c r="Y2" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Z2" s="161"/>
       <c r="AA2" s="9"/>
@@ -7261,16 +7214,16 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="238" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="240" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="240" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="240" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="240" t="s">
-        <v>14</v>
-      </c>
       <c r="D3" s="218" t="s">
-        <v>15</v>
+        <v>126</v>
       </c>
       <c r="E3" s="218"/>
       <c r="F3" s="218"/>
@@ -7282,19 +7235,19 @@
       <c r="L3" s="218"/>
       <c r="M3" s="218"/>
       <c r="N3" s="11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="P3" s="238" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="240" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" s="240" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="240" t="s">
-        <v>13</v>
-      </c>
-      <c r="R3" s="240" t="s">
-        <v>14</v>
-      </c>
       <c r="S3" s="218" t="s">
-        <v>15</v>
+        <v>126</v>
       </c>
       <c r="T3" s="218"/>
       <c r="U3" s="218"/>
@@ -7306,7 +7259,7 @@
       <c r="AA3" s="218"/>
       <c r="AB3" s="218"/>
       <c r="AC3" s="11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
@@ -7341,7 +7294,7 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="242" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" s="243"/>
       <c r="C5" s="244"/>
@@ -7357,7 +7310,7 @@
       <c r="M5" s="14"/>
       <c r="N5" s="13"/>
       <c r="P5" s="219" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="Q5" s="220"/>
       <c r="R5" s="221"/>
@@ -7405,13 +7358,13 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
@@ -7425,13 +7378,13 @@
       <c r="M7" s="20"/>
       <c r="N7" s="21"/>
       <c r="P7" s="15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="Q7" s="18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="R7" s="19" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="S7" s="20"/>
       <c r="T7" s="20"/>
@@ -7442,10 +7395,10 @@
       <c r="Y7" s="20"/>
       <c r="Z7" s="20"/>
       <c r="AA7" s="163" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AB7" s="163" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC7" s="21"/>
     </row>
@@ -7481,13 +7434,13 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
@@ -7501,13 +7454,13 @@
       <c r="M9" s="24"/>
       <c r="N9" s="13"/>
       <c r="P9" s="15" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="Q9" s="22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="R9" s="23" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="S9" s="24"/>
       <c r="T9" s="24"/>
@@ -7524,10 +7477,10 @@
     <row r="10" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="25" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
@@ -7542,10 +7495,10 @@
       <c r="N10" s="13"/>
       <c r="P10" s="15"/>
       <c r="Q10" s="25" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="R10" s="23" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="S10" s="24"/>
       <c r="T10" s="24"/>
@@ -7562,10 +7515,10 @@
     <row r="11" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="22" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>26</v>
+        <v>127</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
@@ -7578,14 +7531,14 @@
       <c r="L11" s="27"/>
       <c r="M11" s="192"/>
       <c r="N11" s="117" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="P11" s="15"/>
       <c r="Q11" s="22" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="R11" s="26" t="s">
-        <v>26</v>
+        <v>128</v>
       </c>
       <c r="S11" s="27"/>
       <c r="T11" s="27"/>
@@ -7602,7 +7555,7 @@
     <row r="12" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
       <c r="B12" s="222" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C12" s="222"/>
       <c r="D12" s="28"/>
@@ -7618,7 +7571,7 @@
       <c r="N12" s="13"/>
       <c r="P12" s="15"/>
       <c r="Q12" s="222" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="R12" s="222"/>
       <c r="S12" s="28"/>
@@ -7636,11 +7589,11 @@
     <row r="13" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="209" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="C13" s="209"/>
       <c r="D13" s="193" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
@@ -7654,7 +7607,7 @@
       <c r="N13" s="13"/>
       <c r="P13" s="15"/>
       <c r="Q13" s="209" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="R13" s="209"/>
       <c r="S13" s="118"/>
@@ -7677,15 +7630,15 @@
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
       <c r="G14" s="31" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H14" s="67"/>
       <c r="I14" s="31" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J14" s="67"/>
       <c r="K14" s="223" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="L14" s="224"/>
       <c r="M14" s="69"/>
@@ -7697,15 +7650,15 @@
       <c r="T14" s="30"/>
       <c r="U14" s="30"/>
       <c r="V14" s="31" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="W14" s="119"/>
       <c r="X14" s="31" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="Y14" s="32"/>
       <c r="Z14" s="223" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="AA14" s="224"/>
       <c r="AB14" s="120"/>
@@ -7719,15 +7672,15 @@
       <c r="E15" s="30"/>
       <c r="F15" s="30"/>
       <c r="G15" s="31" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="H15" s="68"/>
       <c r="I15" s="31" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="J15" s="67"/>
       <c r="K15" s="223" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="L15" s="224"/>
       <c r="M15" s="70"/>
@@ -7739,19 +7692,19 @@
       <c r="T15" s="30"/>
       <c r="U15" s="30"/>
       <c r="V15" s="31" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="W15" s="119"/>
       <c r="X15" s="31" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
       <c r="Y15" s="32"/>
       <c r="Z15" s="223" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="AA15" s="224"/>
       <c r="AB15" s="119" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC15" s="13"/>
     </row>
@@ -7787,13 +7740,13 @@
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B17" s="225" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="D17" s="36"/>
       <c r="E17" s="37"/>
@@ -7805,17 +7758,17 @@
       <c r="K17" s="37"/>
       <c r="L17" s="37"/>
       <c r="M17" s="38" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="N17" s="13"/>
       <c r="P17" s="15" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="Q17" s="225" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="R17" s="35" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="S17" s="37"/>
       <c r="T17" s="37"/>
@@ -7826,10 +7779,10 @@
       <c r="Y17" s="37"/>
       <c r="Z17" s="37"/>
       <c r="AA17" s="166" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AB17" s="167" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC17" s="13"/>
     </row>
@@ -7837,7 +7790,7 @@
       <c r="A18" s="15"/>
       <c r="B18" s="226"/>
       <c r="C18" s="40" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="D18" s="41"/>
       <c r="E18" s="42"/>
@@ -7849,13 +7802,13 @@
       <c r="K18" s="42"/>
       <c r="L18" s="42"/>
       <c r="M18" s="43" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="N18" s="13"/>
       <c r="P18" s="15"/>
       <c r="Q18" s="226"/>
       <c r="R18" s="40" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="S18" s="42"/>
       <c r="T18" s="42"/>
@@ -7866,20 +7819,20 @@
       <c r="Y18" s="42"/>
       <c r="Z18" s="42"/>
       <c r="AA18" s="168" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AB18" s="169" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC18" s="13"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" s="15"/>
       <c r="B19" s="225" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="D19" s="37"/>
       <c r="E19" s="37"/>
@@ -7891,15 +7844,15 @@
       <c r="K19" s="37"/>
       <c r="L19" s="37"/>
       <c r="M19" s="38" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="N19" s="13"/>
       <c r="P19" s="15"/>
       <c r="Q19" s="225" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="R19" s="35" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="S19" s="37"/>
       <c r="T19" s="37"/>
@@ -7910,10 +7863,10 @@
       <c r="Y19" s="37"/>
       <c r="Z19" s="37"/>
       <c r="AA19" s="166" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AB19" s="167" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC19" s="13"/>
     </row>
@@ -7921,7 +7874,7 @@
       <c r="A20" s="15"/>
       <c r="B20" s="226"/>
       <c r="C20" s="40" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="D20" s="42"/>
       <c r="E20" s="42"/>
@@ -7933,13 +7886,13 @@
       <c r="K20" s="42"/>
       <c r="L20" s="42"/>
       <c r="M20" s="43" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="N20" s="13"/>
       <c r="P20" s="15"/>
       <c r="Q20" s="226"/>
       <c r="R20" s="40" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="S20" s="42"/>
       <c r="T20" s="42"/>
@@ -7950,20 +7903,20 @@
       <c r="Y20" s="42"/>
       <c r="Z20" s="42"/>
       <c r="AA20" s="168" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AB20" s="169" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC20" s="13"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" s="15"/>
       <c r="B21" s="225" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>43</v>
+        <v>113</v>
       </c>
       <c r="D21" s="37"/>
       <c r="E21" s="37"/>
@@ -7975,15 +7928,15 @@
       <c r="K21" s="37"/>
       <c r="L21" s="37"/>
       <c r="M21" s="38" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="N21" s="13"/>
       <c r="P21" s="15"/>
       <c r="Q21" s="225" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="R21" s="35" t="s">
-        <v>43</v>
+        <v>113</v>
       </c>
       <c r="S21" s="37"/>
       <c r="T21" s="37"/>
@@ -7994,10 +7947,10 @@
       <c r="Y21" s="37"/>
       <c r="Z21" s="37"/>
       <c r="AA21" s="166" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AB21" s="167" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC21" s="13"/>
     </row>
@@ -8005,7 +7958,7 @@
       <c r="A22" s="15"/>
       <c r="B22" s="227"/>
       <c r="C22" s="26" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
@@ -8017,13 +7970,13 @@
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
       <c r="M22" s="45" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="N22" s="13"/>
       <c r="P22" s="15"/>
       <c r="Q22" s="227"/>
       <c r="R22" s="26" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="S22" s="14"/>
       <c r="T22" s="14"/>
@@ -8034,10 +7987,10 @@
       <c r="Y22" s="14"/>
       <c r="Z22" s="14"/>
       <c r="AA22" s="1" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AB22" s="170" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC22" s="13"/>
     </row>
@@ -8045,7 +7998,7 @@
       <c r="A23" s="15"/>
       <c r="B23" s="226"/>
       <c r="C23" s="40" t="s">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="D23" s="42"/>
       <c r="E23" s="42"/>
@@ -8057,13 +8010,13 @@
       <c r="K23" s="42"/>
       <c r="L23" s="42"/>
       <c r="M23" s="43" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="N23" s="13"/>
       <c r="P23" s="15"/>
       <c r="Q23" s="226"/>
       <c r="R23" s="40" t="s">
-        <v>45</v>
+        <v>115</v>
       </c>
       <c r="S23" s="42"/>
       <c r="T23" s="42"/>
@@ -8074,20 +8027,20 @@
       <c r="Y23" s="42"/>
       <c r="Z23" s="42"/>
       <c r="AA23" s="168" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AB23" s="169" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC23" s="13"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24" s="15"/>
       <c r="B24" s="225" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C24" s="35" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
       <c r="D24" s="37"/>
       <c r="E24" s="37"/>
@@ -8099,15 +8052,15 @@
       <c r="K24" s="37"/>
       <c r="L24" s="37"/>
       <c r="M24" s="38" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="N24" s="13"/>
       <c r="P24" s="15"/>
       <c r="Q24" s="225" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="R24" s="35" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
       <c r="S24" s="37"/>
       <c r="T24" s="37"/>
@@ -8118,10 +8071,10 @@
       <c r="Y24" s="37"/>
       <c r="Z24" s="37"/>
       <c r="AA24" s="166" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AB24" s="167" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC24" s="13"/>
     </row>
@@ -8129,7 +8082,7 @@
       <c r="A25" s="15"/>
       <c r="B25" s="227"/>
       <c r="C25" s="26" t="s">
-        <v>48</v>
+        <v>117</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
@@ -8141,13 +8094,13 @@
       <c r="K25" s="14"/>
       <c r="L25" s="14"/>
       <c r="M25" s="45" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="N25" s="13"/>
       <c r="P25" s="15"/>
       <c r="Q25" s="227"/>
       <c r="R25" s="26" t="s">
-        <v>48</v>
+        <v>117</v>
       </c>
       <c r="S25" s="14"/>
       <c r="T25" s="14"/>
@@ -8158,10 +8111,10 @@
       <c r="Y25" s="14"/>
       <c r="Z25" s="14"/>
       <c r="AA25" s="1" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AB25" s="170" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC25" s="13"/>
     </row>
@@ -8169,7 +8122,7 @@
       <c r="A26" s="15"/>
       <c r="B26" s="226"/>
       <c r="C26" s="40" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="D26" s="42"/>
       <c r="E26" s="42"/>
@@ -8181,13 +8134,13 @@
       <c r="K26" s="42"/>
       <c r="L26" s="42"/>
       <c r="M26" s="43" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="N26" s="13"/>
       <c r="P26" s="15"/>
       <c r="Q26" s="226"/>
       <c r="R26" s="40" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="S26" s="42"/>
       <c r="T26" s="42"/>
@@ -8198,10 +8151,10 @@
       <c r="Y26" s="42"/>
       <c r="Z26" s="42"/>
       <c r="AA26" s="168" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AB26" s="169" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC26" s="13"/>
     </row>
@@ -8209,7 +8162,7 @@
       <c r="A27" s="15"/>
       <c r="B27" s="34"/>
       <c r="C27" s="35" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="D27" s="37"/>
       <c r="E27" s="37"/>
@@ -8221,15 +8174,15 @@
       <c r="K27" s="37"/>
       <c r="L27" s="37"/>
       <c r="M27" s="38" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="N27" s="13"/>
       <c r="P27" s="15"/>
       <c r="Q27" s="228" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="R27" s="35" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="S27" s="37"/>
       <c r="T27" s="37"/>
@@ -8240,20 +8193,20 @@
       <c r="Y27" s="37"/>
       <c r="Z27" s="37"/>
       <c r="AA27" s="166" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AB27" s="167" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC27" s="13"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28" s="15"/>
       <c r="B28" s="44" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
@@ -8265,13 +8218,13 @@
       <c r="K28" s="14"/>
       <c r="L28" s="14"/>
       <c r="M28" s="45" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="N28" s="13"/>
       <c r="P28" s="15"/>
       <c r="Q28" s="229"/>
       <c r="R28" s="26" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="S28" s="14"/>
       <c r="T28" s="14"/>
@@ -8282,10 +8235,10 @@
       <c r="Y28" s="14"/>
       <c r="Z28" s="14"/>
       <c r="AA28" s="1" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AB28" s="170" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC28" s="13"/>
     </row>
@@ -8293,7 +8246,7 @@
       <c r="A29" s="15"/>
       <c r="B29" s="39"/>
       <c r="C29" s="40" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="D29" s="42"/>
       <c r="E29" s="42"/>
@@ -8305,13 +8258,13 @@
       <c r="K29" s="42"/>
       <c r="L29" s="42"/>
       <c r="M29" s="43" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="N29" s="13"/>
       <c r="P29" s="15"/>
       <c r="Q29" s="230"/>
       <c r="R29" s="40" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="S29" s="42"/>
       <c r="T29" s="42"/>
@@ -8322,20 +8275,20 @@
       <c r="Y29" s="42"/>
       <c r="Z29" s="42"/>
       <c r="AA29" s="168" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AB29" s="169" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC29" s="13"/>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30" s="15"/>
       <c r="B30" s="215" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="D30" s="37"/>
       <c r="E30" s="37"/>
@@ -8347,15 +8300,15 @@
       <c r="K30" s="37"/>
       <c r="L30" s="37"/>
       <c r="M30" s="38" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="N30" s="13"/>
       <c r="P30" s="15"/>
       <c r="Q30" s="215" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="R30" s="35" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="S30" s="37"/>
       <c r="T30" s="37"/>
@@ -8366,10 +8319,10 @@
       <c r="Y30" s="37"/>
       <c r="Z30" s="37"/>
       <c r="AA30" s="166" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AB30" s="167" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC30" s="13"/>
     </row>
@@ -8377,7 +8330,7 @@
       <c r="A31" s="15"/>
       <c r="B31" s="216"/>
       <c r="C31" s="26" t="s">
-        <v>56</v>
+        <v>123</v>
       </c>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
@@ -8389,13 +8342,13 @@
       <c r="K31" s="14"/>
       <c r="L31" s="14"/>
       <c r="M31" s="45" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="N31" s="46"/>
       <c r="P31" s="15"/>
       <c r="Q31" s="216"/>
       <c r="R31" s="26" t="s">
-        <v>56</v>
+        <v>123</v>
       </c>
       <c r="S31" s="14"/>
       <c r="T31" s="14"/>
@@ -8406,10 +8359,10 @@
       <c r="Y31" s="14"/>
       <c r="Z31" s="14"/>
       <c r="AA31" s="1" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AB31" s="170" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC31" s="46"/>
     </row>
@@ -8417,7 +8370,7 @@
       <c r="A32" s="15"/>
       <c r="B32" s="217"/>
       <c r="C32" s="40" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="D32" s="42"/>
       <c r="E32" s="42"/>
@@ -8429,13 +8382,13 @@
       <c r="K32" s="42"/>
       <c r="L32" s="42"/>
       <c r="M32" s="43" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="N32" s="13"/>
       <c r="P32" s="15"/>
       <c r="Q32" s="217"/>
       <c r="R32" s="40" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="S32" s="42"/>
       <c r="T32" s="42"/>
@@ -8446,17 +8399,17 @@
       <c r="Y32" s="42"/>
       <c r="Z32" s="42"/>
       <c r="AA32" s="168" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AB32" s="169" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="AC32" s="13"/>
     </row>
     <row r="33" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
       <c r="B33" s="209" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="C33" s="210"/>
       <c r="D33" s="47"/>
@@ -8472,7 +8425,7 @@
       <c r="N33" s="13"/>
       <c r="P33" s="15"/>
       <c r="Q33" s="209" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="R33" s="210"/>
       <c r="S33" s="47"/>
@@ -8490,7 +8443,7 @@
     <row r="34" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
       <c r="B34" s="209" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="C34" s="209"/>
       <c r="D34" s="48"/>
@@ -8504,11 +8457,11 @@
       <c r="L34" s="48"/>
       <c r="M34" s="49"/>
       <c r="N34" s="117" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="P34" s="15"/>
       <c r="Q34" s="209" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="R34" s="209"/>
       <c r="S34" s="48"/>
@@ -8526,7 +8479,7 @@
     <row r="35" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
       <c r="B35" s="209" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="C35" s="210"/>
       <c r="D35" s="28"/>
@@ -8542,7 +8495,7 @@
       <c r="N35" s="13"/>
       <c r="P35" s="15"/>
       <c r="Q35" s="209" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="R35" s="210"/>
       <c r="S35" s="28"/>
@@ -8560,11 +8513,11 @@
     <row r="36" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
       <c r="B36" s="209" t="s">
-        <v>61</v>
+        <v>125</v>
       </c>
       <c r="C36" s="209"/>
       <c r="D36" s="193" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E36" s="17"/>
       <c r="F36" s="17"/>
@@ -8578,7 +8531,7 @@
       <c r="N36" s="13"/>
       <c r="P36" s="15"/>
       <c r="Q36" s="209" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="R36" s="209"/>
       <c r="S36" s="121"/>
@@ -8626,7 +8579,7 @@
     <row r="38" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="50"/>
       <c r="B38" s="16" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="C38" s="16"/>
       <c r="D38" s="48"/>
@@ -8640,11 +8593,11 @@
       <c r="L38" s="48"/>
       <c r="M38" s="49"/>
       <c r="N38" s="117" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="P38" s="50"/>
       <c r="Q38" s="16" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="R38" s="16"/>
       <c r="S38" s="48"/>
@@ -8662,7 +8615,7 @@
     <row r="39" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A39" s="50"/>
       <c r="B39" s="16" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="C39" s="51"/>
       <c r="D39" s="1"/>
@@ -8678,7 +8631,7 @@
       <c r="N39" s="13"/>
       <c r="P39" s="50"/>
       <c r="Q39" s="16" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="R39" s="51"/>
       <c r="S39" s="122"/>
@@ -8726,40 +8679,40 @@
     <row r="41" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="52"/>
       <c r="B41" s="211" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C41" s="212"/>
       <c r="D41" s="54" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
       <c r="I41" s="9" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="J41" s="9"/>
       <c r="K41" s="194" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="L41" s="9"/>
       <c r="M41" s="9"/>
       <c r="N41" s="10"/>
       <c r="P41" s="52"/>
       <c r="Q41" s="211" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="R41" s="212"/>
       <c r="S41" s="54" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="T41" s="9"/>
       <c r="U41" s="9"/>
       <c r="V41" s="9"/>
       <c r="W41" s="9"/>
       <c r="X41" s="9" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="Y41" s="9"/>
       <c r="Z41" s="123"/>
@@ -8770,7 +8723,7 @@
     <row r="42" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A42" s="52"/>
       <c r="B42" s="213" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="C42" s="214"/>
       <c r="D42" s="55"/>
@@ -8786,7 +8739,7 @@
       <c r="N42" s="10"/>
       <c r="P42" s="52"/>
       <c r="Q42" s="213" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="R42" s="214"/>
       <c r="S42" s="55"/>
@@ -8804,7 +8757,7 @@
     <row r="43" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A43" s="52"/>
       <c r="B43" s="205" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="C43" s="206"/>
       <c r="D43" s="56">
@@ -8822,7 +8775,7 @@
       <c r="N43" s="10"/>
       <c r="P43" s="52"/>
       <c r="Q43" s="205" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="R43" s="206"/>
       <c r="S43" s="56">
@@ -8842,7 +8795,7 @@
     <row r="44" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A44" s="52"/>
       <c r="B44" s="205" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C44" s="206"/>
       <c r="D44" s="57">
@@ -8860,7 +8813,7 @@
       <c r="N44" s="10"/>
       <c r="P44" s="52"/>
       <c r="Q44" s="205" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="R44" s="206"/>
       <c r="S44" s="57">
@@ -8880,7 +8833,7 @@
     <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45" s="52"/>
       <c r="B45" s="205" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="C45" s="206"/>
       <c r="D45" s="58">
@@ -8898,7 +8851,7 @@
       <c r="N45" s="59"/>
       <c r="P45" s="52"/>
       <c r="Q45" s="205" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="R45" s="206"/>
       <c r="S45" s="58">
@@ -8918,7 +8871,7 @@
     <row r="46" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A46" s="52"/>
       <c r="B46" s="207" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="C46" s="208"/>
       <c r="D46" s="60">
@@ -8936,7 +8889,7 @@
       <c r="N46" s="59"/>
       <c r="P46" s="52"/>
       <c r="Q46" s="207" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="R46" s="208"/>
       <c r="S46" s="60">
@@ -8985,7 +8938,7 @@
     </row>
     <row r="50" spans="6:14" ht="20" x14ac:dyDescent="0.25">
       <c r="F50" s="64" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="I50" s="65"/>
       <c r="N50" s="66"/>
@@ -9942,11 +9895,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C7B2D4-D38D-4D01-9B83-C70548CD7D94}">
   <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="S1" zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26:O26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="11" style="64"/>
     <col min="4" max="4" width="12" style="64" customWidth="1"/>
@@ -9956,36 +9909,36 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="71" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" s="233"/>
       <c r="E1" s="233"/>
       <c r="F1" s="233"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I1" s="268"/>
       <c r="J1" s="268"/>
       <c r="K1" s="72"/>
       <c r="L1" s="99"/>
       <c r="N1" s="71" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="O1" s="4"/>
       <c r="P1" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="Q1" s="233"/>
       <c r="R1" s="233"/>
       <c r="S1" s="233"/>
       <c r="T1" s="4"/>
       <c r="U1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="V1" s="268"/>
       <c r="W1" s="268"/>
@@ -9994,36 +9947,36 @@
     </row>
     <row r="2" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="269"/>
       <c r="E2" s="269"/>
       <c r="F2" s="269"/>
       <c r="G2" s="9"/>
       <c r="H2" s="9" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="I2" s="162"/>
       <c r="J2" s="73"/>
       <c r="K2" s="73"/>
       <c r="L2" s="100"/>
       <c r="N2" s="52" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="O2" s="9"/>
       <c r="P2" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q2" s="269"/>
       <c r="R2" s="269"/>
       <c r="S2" s="269"/>
       <c r="T2" s="9"/>
       <c r="U2" s="9" t="s">
-        <v>104</v>
+        <v>9</v>
       </c>
       <c r="V2" s="162"/>
       <c r="W2" s="73"/>
@@ -10032,11 +9985,11 @@
     </row>
     <row r="3" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="270" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="B3" s="271"/>
       <c r="C3" s="274" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="D3" s="274"/>
       <c r="E3" s="274"/>
@@ -10048,11 +10001,11 @@
       <c r="K3" s="274"/>
       <c r="L3" s="275"/>
       <c r="N3" s="270" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="O3" s="271"/>
       <c r="P3" s="274" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="Q3" s="274"/>
       <c r="R3" s="274"/>
@@ -10092,7 +10045,7 @@
     </row>
     <row r="5" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="259" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="B5" s="260"/>
       <c r="C5" s="77"/>
@@ -10106,7 +10059,7 @@
       <c r="K5" s="79"/>
       <c r="L5" s="110"/>
       <c r="N5" s="276" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="O5" s="277"/>
       <c r="P5" s="102"/>
@@ -10122,7 +10075,7 @@
     </row>
     <row r="6" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="259" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="B6" s="260"/>
       <c r="C6" s="80"/>
@@ -10136,7 +10089,7 @@
       <c r="K6" s="82"/>
       <c r="L6" s="111"/>
       <c r="N6" s="276" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="O6" s="277"/>
       <c r="P6" s="84"/>
@@ -10152,7 +10105,7 @@
     </row>
     <row r="7" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="259" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="B7" s="260"/>
       <c r="C7" s="80"/>
@@ -10166,7 +10119,7 @@
       <c r="K7" s="81"/>
       <c r="L7" s="106"/>
       <c r="N7" s="278" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="O7" s="279"/>
       <c r="P7" s="84"/>
@@ -10182,7 +10135,7 @@
     </row>
     <row r="8" spans="1:25" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="284" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="B8" s="285"/>
       <c r="C8" s="83"/>
@@ -10196,7 +10149,7 @@
       <c r="K8" s="84"/>
       <c r="L8" s="113"/>
       <c r="N8" s="257" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="O8" s="258"/>
       <c r="P8" s="83"/>
@@ -10208,15 +10161,15 @@
       <c r="V8" s="84"/>
       <c r="W8" s="84"/>
       <c r="X8" s="138" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Y8" s="139" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="259" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="B9" s="260"/>
       <c r="C9" s="85"/>
@@ -10230,45 +10183,45 @@
       <c r="K9" s="86"/>
       <c r="L9" s="114"/>
       <c r="N9" s="259" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="O9" s="260"/>
       <c r="P9" s="85" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Q9" s="86" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="R9" s="86" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="S9" s="86" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="T9" s="86" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="U9" s="86" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="V9" s="86" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="W9" s="86" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="X9" s="140" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Y9" s="141" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="286"/>
       <c r="B10" s="287"/>
       <c r="C10" s="261" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="D10" s="261"/>
       <c r="E10" s="261"/>
@@ -10282,7 +10235,7 @@
       <c r="N10" s="115"/>
       <c r="O10" s="116"/>
       <c r="P10" s="261" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="Q10" s="261"/>
       <c r="R10" s="261"/>
@@ -10296,10 +10249,10 @@
     </row>
     <row r="11" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="263" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B11" s="76" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C11" s="77"/>
       <c r="D11" s="79"/>
@@ -10312,10 +10265,10 @@
       <c r="K11" s="79"/>
       <c r="L11" s="110"/>
       <c r="N11" s="263" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="O11" s="76" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="P11" s="77"/>
       <c r="Q11" s="79"/>
@@ -10326,16 +10279,16 @@
       <c r="V11" s="79"/>
       <c r="W11" s="79"/>
       <c r="X11" s="142" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Y11" s="143" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="264"/>
       <c r="B12" s="76" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="C12" s="87"/>
       <c r="D12" s="82"/>
@@ -10349,7 +10302,7 @@
       <c r="L12" s="111"/>
       <c r="N12" s="264"/>
       <c r="O12" s="76" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="P12" s="87"/>
       <c r="Q12" s="82"/>
@@ -10360,16 +10313,16 @@
       <c r="V12" s="82"/>
       <c r="W12" s="82"/>
       <c r="X12" s="144" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Y12" s="145" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="264"/>
       <c r="B13" s="76" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="C13" s="87"/>
       <c r="D13" s="82"/>
@@ -10383,7 +10336,7 @@
       <c r="L13" s="111"/>
       <c r="N13" s="264"/>
       <c r="O13" s="76" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="P13" s="87"/>
       <c r="Q13" s="82"/>
@@ -10394,16 +10347,16 @@
       <c r="V13" s="82"/>
       <c r="W13" s="82"/>
       <c r="X13" s="144" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Y13" s="145" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="264"/>
       <c r="B14" s="76" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="C14" s="87"/>
       <c r="D14" s="82"/>
@@ -10417,7 +10370,7 @@
       <c r="L14" s="111"/>
       <c r="N14" s="264"/>
       <c r="O14" s="76" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="P14" s="87"/>
       <c r="Q14" s="82"/>
@@ -10428,16 +10381,16 @@
       <c r="V14" s="82"/>
       <c r="W14" s="82"/>
       <c r="X14" s="144" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Y14" s="145" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="265"/>
       <c r="B15" s="76" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="C15" s="87"/>
       <c r="D15" s="82"/>
@@ -10451,7 +10404,7 @@
       <c r="L15" s="111"/>
       <c r="N15" s="265"/>
       <c r="O15" s="76" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="P15" s="87"/>
       <c r="Q15" s="82"/>
@@ -10462,15 +10415,15 @@
       <c r="V15" s="82"/>
       <c r="W15" s="82"/>
       <c r="X15" s="144" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Y15" s="145" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="259" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="B16" s="260"/>
       <c r="C16" s="87"/>
@@ -10484,7 +10437,7 @@
       <c r="K16" s="82"/>
       <c r="L16" s="111"/>
       <c r="N16" s="259" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="O16" s="260"/>
       <c r="P16" s="87"/>
@@ -10496,15 +10449,15 @@
       <c r="V16" s="82"/>
       <c r="W16" s="82"/>
       <c r="X16" s="144" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Y16" s="145" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="259" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="B17" s="260"/>
       <c r="C17" s="88"/>
@@ -10518,7 +10471,7 @@
       <c r="K17" s="89"/>
       <c r="L17" s="112"/>
       <c r="N17" s="259" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="O17" s="260"/>
       <c r="P17" s="88"/>
@@ -10530,17 +10483,17 @@
       <c r="V17" s="89"/>
       <c r="W17" s="89"/>
       <c r="X17" s="146" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Y17" s="147" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="282"/>
       <c r="B18" s="283"/>
       <c r="C18" s="253" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="D18" s="253"/>
       <c r="E18" s="253"/>
@@ -10554,7 +10507,7 @@
       <c r="N18" s="52"/>
       <c r="O18" s="9"/>
       <c r="P18" s="253" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="Q18" s="253"/>
       <c r="R18" s="253"/>
@@ -10568,7 +10521,7 @@
     </row>
     <row r="19" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="247" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="B19" s="248"/>
       <c r="C19" s="77"/>
@@ -10582,7 +10535,7 @@
       <c r="K19" s="92"/>
       <c r="L19" s="105"/>
       <c r="N19" s="247" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="O19" s="248"/>
       <c r="P19" s="77"/>
@@ -10594,15 +10547,15 @@
       <c r="V19" s="92"/>
       <c r="W19" s="92"/>
       <c r="X19" s="148" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Y19" s="149" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="247" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
       <c r="B20" s="248"/>
       <c r="C20" s="87"/>
@@ -10616,7 +10569,7 @@
       <c r="K20" s="81"/>
       <c r="L20" s="106"/>
       <c r="N20" s="247" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
       <c r="O20" s="248"/>
       <c r="P20" s="87"/>
@@ -10628,15 +10581,15 @@
       <c r="V20" s="81"/>
       <c r="W20" s="81"/>
       <c r="X20" s="150" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Y20" s="151" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="247" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="B21" s="248"/>
       <c r="C21" s="87"/>
@@ -10650,7 +10603,7 @@
       <c r="K21" s="81"/>
       <c r="L21" s="106"/>
       <c r="N21" s="247" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="O21" s="248"/>
       <c r="P21" s="87"/>
@@ -10662,15 +10615,15 @@
       <c r="V21" s="81"/>
       <c r="W21" s="81"/>
       <c r="X21" s="150" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Y21" s="151" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="247" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="B22" s="248"/>
       <c r="C22" s="87"/>
@@ -10684,7 +10637,7 @@
       <c r="K22" s="81"/>
       <c r="L22" s="106"/>
       <c r="N22" s="247" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
       <c r="O22" s="248"/>
       <c r="P22" s="87"/>
@@ -10696,18 +10649,18 @@
       <c r="V22" s="81"/>
       <c r="W22" s="81"/>
       <c r="X22" s="150" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Y22" s="151" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="132" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="B23" s="133" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="C23" s="93"/>
       <c r="D23" s="94"/>
@@ -10720,10 +10673,10 @@
       <c r="K23" s="94"/>
       <c r="L23" s="107"/>
       <c r="N23" s="90" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="O23" s="91" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="P23" s="93"/>
       <c r="Q23" s="94"/>
@@ -10738,7 +10691,7 @@
     </row>
     <row r="24" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="255" t="s">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="B24" s="256"/>
       <c r="C24" s="87"/>
@@ -10752,7 +10705,7 @@
       <c r="K24" s="81"/>
       <c r="L24" s="106"/>
       <c r="N24" s="255" t="s">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="O24" s="256"/>
       <c r="P24" s="87"/>
@@ -10764,15 +10717,15 @@
       <c r="V24" s="81"/>
       <c r="W24" s="81"/>
       <c r="X24" s="150" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Y24" s="151" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="249" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="B25" s="250"/>
       <c r="C25" s="87"/>
@@ -10786,7 +10739,7 @@
       <c r="K25" s="81"/>
       <c r="L25" s="106"/>
       <c r="N25" s="247" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="O25" s="248"/>
       <c r="P25" s="87"/>
@@ -10798,15 +10751,15 @@
       <c r="V25" s="81"/>
       <c r="W25" s="81"/>
       <c r="X25" s="150" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Y25" s="151" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="280" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="B26" s="281"/>
       <c r="C26" s="95"/>
@@ -10820,7 +10773,7 @@
       <c r="K26" s="96"/>
       <c r="L26" s="108"/>
       <c r="N26" s="249" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="O26" s="250"/>
       <c r="P26" s="95"/>
@@ -10832,15 +10785,15 @@
       <c r="V26" s="96"/>
       <c r="W26" s="96"/>
       <c r="X26" s="154" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Y26" s="155" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:25" ht="83.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="251" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="B27" s="266"/>
       <c r="C27" s="97"/>
@@ -10854,7 +10807,7 @@
       <c r="K27" s="98"/>
       <c r="L27" s="109"/>
       <c r="N27" s="251" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="O27" s="252"/>
       <c r="P27" s="98"/>
@@ -10866,10 +10819,10 @@
       <c r="V27" s="98"/>
       <c r="W27" s="98"/>
       <c r="X27" s="156" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="Y27" s="157" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
@@ -10937,10 +10890,10 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="24" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="183"/>
     <col min="2" max="3" width="36.33203125" style="186" customWidth="1"/>
@@ -10950,7 +10903,7 @@
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="288" t="s">
-        <v>138</v>
+        <v>99</v>
       </c>
       <c r="B2" s="288"/>
       <c r="C2" s="288"/>
@@ -10977,13 +10930,13 @@
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="185" t="s">
-        <v>136</v>
+        <v>94</v>
       </c>
       <c r="B5" s="188" t="s">
-        <v>137</v>
+        <v>98</v>
       </c>
       <c r="C5" s="188" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="281" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11014,44 +10967,29 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0128B0-B87E-4E33-8001-348F9AE9F653}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ADD94E2-FB59-6042-8742-8260D104F858}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>